<commit_message>
Kleinere Änderungen im Kopf etc.
</commit_message>
<xml_diff>
--- a/addtotoc_helper.xlsx
+++ b/addtotoc_helper.xlsx
@@ -9,12 +9,11 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20025" windowHeight="9555" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20025" windowHeight="9555" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="DIN V 18599 Berechnungsunterlag" sheetId="1" r:id="rId1"/>
     <sheet name="DIN V 18599 Berechnungsungs REF" sheetId="2" r:id="rId2"/>
-    <sheet name="DIN V 18599 Berechnungsungs (2" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -26,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="405" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="274" uniqueCount="52">
   <si>
     <t>chapter</t>
   </si>
@@ -549,8 +548,8 @@
         <v>2</v>
       </c>
       <c r="F4" t="str">
-        <f t="shared" ref="F4:F67" si="0">CONCATENATE(D4,", ",IF(ISBLANK(A4)=FALSE,A$3,IF(ISBLANK(B4)=FALSE,B$3,C$3)),", ",IF(ISBLANK(A4)=FALSE,0,IF(ISBLANK(B4)=FALSE,1,2)),", ",IF(ISBLANK(A4)=FALSE,A4,IF(ISBLANK(B4)=FALSE,B4,C4)),IF(ISBLANK(D5)=TRUE,",",", ,"))</f>
-        <v>2, section, 1, Allgemeine Angaben zum Gebäude, ,</v>
+        <f>CONCATENATE(D4,", ",IF(ISBLANK(A4)=FALSE,A$3,IF(ISBLANK(B4)=FALSE,B$3,C$3)),", ",IF(ISBLANK(A4)=FALSE,0,IF(ISBLANK(B4)=FALSE,1,2)),", {",IF(ISBLANK(A4)=FALSE,A4,IF(ISBLANK(B4)=FALSE,B4,C4)),"}, a",IF(ISBLANK(D5)=TRUE,"",","))</f>
+        <v>2, section, 1, {Allgemeine Angaben zum Gebäude}, a,</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
@@ -561,8 +560,8 @@
         <v>3</v>
       </c>
       <c r="F5" t="str">
-        <f t="shared" si="0"/>
-        <v>3, subsection, 2, Zonen, ,</v>
+        <f t="shared" ref="F5:F68" si="0">CONCATENATE(D5,", ",IF(ISBLANK(A5)=FALSE,A$3,IF(ISBLANK(B5)=FALSE,B$3,C$3)),", ",IF(ISBLANK(A5)=FALSE,0,IF(ISBLANK(B5)=FALSE,1,2)),", {",IF(ISBLANK(A5)=FALSE,A5,IF(ISBLANK(B5)=FALSE,B5,C5)),"}, a",IF(ISBLANK(D6)=TRUE,"",","))</f>
+        <v>3, subsection, 2, {Zonen}, a,</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
@@ -574,7 +573,7 @@
       </c>
       <c r="F6" t="str">
         <f t="shared" si="0"/>
-        <v>4, subsection, 2, Hüllfläche, ,</v>
+        <v>4, subsection, 2, {Hüllfläche}, a,</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
@@ -586,7 +585,7 @@
       </c>
       <c r="F7" t="str">
         <f t="shared" si="0"/>
-        <v>7, subsection, 2, Bauteilflächen, ,</v>
+        <v>7, subsection, 2, {Bauteilflächen}, a,</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
@@ -598,7 +597,7 @@
       </c>
       <c r="F8" t="str">
         <f t="shared" si="0"/>
-        <v>11, subsection, 2, Raumliste, ,</v>
+        <v>11, subsection, 2, {Raumliste}, a,</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
@@ -610,7 +609,7 @@
       </c>
       <c r="F9" t="str">
         <f t="shared" si="0"/>
-        <v>12, subsection, 2, Energiebilanz, ,</v>
+        <v>12, subsection, 2, {Energiebilanz}, a,</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
@@ -622,7 +621,7 @@
       </c>
       <c r="F10" t="str">
         <f t="shared" si="0"/>
-        <v>18, section, 1, Bewertung des Gebäudes entsprechend den GEG-Anforderungen, ,</v>
+        <v>18, section, 1, {Bewertung des Gebäudes entsprechend den GEG-Anforderungen}, a,</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
@@ -634,7 +633,7 @@
       </c>
       <c r="F11" t="str">
         <f t="shared" si="0"/>
-        <v>19, section, 1, Zone Verkaufsraum, ,</v>
+        <v>19, section, 1, {Zone Verkaufsraum}, a,</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
@@ -646,7 +645,7 @@
       </c>
       <c r="F12" t="str">
         <f t="shared" si="0"/>
-        <v>19, subsection, 2, Geometrie, ,</v>
+        <v>19, subsection, 2, {Geometrie}, a,</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
@@ -658,7 +657,7 @@
       </c>
       <c r="F13" t="str">
         <f t="shared" si="0"/>
-        <v>19, subsection, 2, Hüllfläche, ,</v>
+        <v>19, subsection, 2, {Hüllfläche}, a,</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
@@ -670,7 +669,7 @@
       </c>
       <c r="F14" t="str">
         <f t="shared" si="0"/>
-        <v>21, subsection, 2, Raumliste, ,</v>
+        <v>21, subsection, 2, {Raumliste}, a,</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
@@ -682,7 +681,7 @@
       </c>
       <c r="F15" t="str">
         <f t="shared" si="0"/>
-        <v>21, subsection, 2, Randbedingungen, ,</v>
+        <v>21, subsection, 2, {Randbedingungen}, a,</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
@@ -694,7 +693,7 @@
       </c>
       <c r="F16" t="str">
         <f t="shared" si="0"/>
-        <v>21, subsection, 2, Luftwechsel, ,</v>
+        <v>21, subsection, 2, {Luftwechsel}, a,</v>
       </c>
     </row>
     <row r="17" spans="2:6" x14ac:dyDescent="0.25">
@@ -706,7 +705,7 @@
       </c>
       <c r="F17" t="str">
         <f t="shared" si="0"/>
-        <v>21, subsection, 2, Nutzungszeiten, ,</v>
+        <v>21, subsection, 2, {Nutzungszeiten}, a,</v>
       </c>
     </row>
     <row r="18" spans="2:6" x14ac:dyDescent="0.25">
@@ -718,7 +717,7 @@
       </c>
       <c r="F18" t="str">
         <f t="shared" si="0"/>
-        <v>21, subsection, 2, Heizung, ,</v>
+        <v>21, subsection, 2, {Heizung}, a,</v>
       </c>
     </row>
     <row r="19" spans="2:6" x14ac:dyDescent="0.25">
@@ -730,7 +729,7 @@
       </c>
       <c r="F19" t="str">
         <f t="shared" si="0"/>
-        <v>22, subsection, 2, Kühlung, ,</v>
+        <v>22, subsection, 2, {Kühlung}, a,</v>
       </c>
     </row>
     <row r="20" spans="2:6" x14ac:dyDescent="0.25">
@@ -742,7 +741,7 @@
       </c>
       <c r="F20" t="str">
         <f t="shared" si="0"/>
-        <v>22, subsection, 2, Lüftung, ,</v>
+        <v>22, subsection, 2, {Lüftung}, a,</v>
       </c>
     </row>
     <row r="21" spans="2:6" x14ac:dyDescent="0.25">
@@ -754,7 +753,7 @@
       </c>
       <c r="F21" t="str">
         <f t="shared" si="0"/>
-        <v>22, subsection, 2, Beleuchtung, ,</v>
+        <v>22, subsection, 2, {Beleuchtung}, a,</v>
       </c>
     </row>
     <row r="22" spans="2:6" x14ac:dyDescent="0.25">
@@ -766,7 +765,7 @@
       </c>
       <c r="F22" t="str">
         <f t="shared" si="0"/>
-        <v>22, subsection, 2, Wärmequellen, ,</v>
+        <v>22, subsection, 2, {Wärmequellen}, a,</v>
       </c>
     </row>
     <row r="23" spans="2:6" x14ac:dyDescent="0.25">
@@ -778,7 +777,7 @@
       </c>
       <c r="F23" t="str">
         <f t="shared" si="0"/>
-        <v>22, subsection, 2, Trinkwarmwasser, ,</v>
+        <v>22, subsection, 2, {Trinkwarmwasser}, a,</v>
       </c>
     </row>
     <row r="24" spans="2:6" x14ac:dyDescent="0.25">
@@ -790,7 +789,7 @@
       </c>
       <c r="F24" t="str">
         <f t="shared" si="0"/>
-        <v>22, subsection, 2, Gezielter Luftaustausch mit Zone Pfangutlager, ,</v>
+        <v>22, subsection, 2, {Gezielter Luftaustausch mit Zone Pfangutlager}, a,</v>
       </c>
     </row>
     <row r="25" spans="2:6" x14ac:dyDescent="0.25">
@@ -802,7 +801,7 @@
       </c>
       <c r="F25" t="str">
         <f t="shared" si="0"/>
-        <v>23, subsection, 2, Konfiguration Lüftungsanlage, ,</v>
+        <v>23, subsection, 2, {Konfiguration Lüftungsanlage}, a,</v>
       </c>
     </row>
     <row r="26" spans="2:6" x14ac:dyDescent="0.25">
@@ -814,7 +813,7 @@
       </c>
       <c r="F26" t="str">
         <f t="shared" si="0"/>
-        <v>30, subsection, 2, Berechnung / Ergebnisse, ,</v>
+        <v>30, subsection, 2, {Berechnung / Ergebnisse}, a,</v>
       </c>
     </row>
     <row r="27" spans="2:6" x14ac:dyDescent="0.25">
@@ -826,7 +825,7 @@
       </c>
       <c r="F27" t="str">
         <f t="shared" si="0"/>
-        <v>33, section, 1, Zone Lager, ,</v>
+        <v>33, section, 1, {Zone Lager}, a,</v>
       </c>
     </row>
     <row r="28" spans="2:6" x14ac:dyDescent="0.25">
@@ -838,7 +837,7 @@
       </c>
       <c r="F28" t="str">
         <f t="shared" si="0"/>
-        <v>33, subsection, 2, Geometrie, ,</v>
+        <v>33, subsection, 2, {Geometrie}, a,</v>
       </c>
     </row>
     <row r="29" spans="2:6" x14ac:dyDescent="0.25">
@@ -850,7 +849,7 @@
       </c>
       <c r="F29" t="str">
         <f t="shared" si="0"/>
-        <v>33, subsection, 2, Hüllfläche, ,</v>
+        <v>33, subsection, 2, {Hüllfläche}, a,</v>
       </c>
     </row>
     <row r="30" spans="2:6" x14ac:dyDescent="0.25">
@@ -862,7 +861,7 @@
       </c>
       <c r="F30" t="str">
         <f t="shared" si="0"/>
-        <v>35, subsection, 2, Raumliste, ,</v>
+        <v>35, subsection, 2, {Raumliste}, a,</v>
       </c>
     </row>
     <row r="31" spans="2:6" x14ac:dyDescent="0.25">
@@ -874,7 +873,7 @@
       </c>
       <c r="F31" t="str">
         <f t="shared" si="0"/>
-        <v>35, subsection, 2, Randbedingungen, ,</v>
+        <v>35, subsection, 2, {Randbedingungen}, a,</v>
       </c>
     </row>
     <row r="32" spans="2:6" x14ac:dyDescent="0.25">
@@ -886,7 +885,7 @@
       </c>
       <c r="F32" t="str">
         <f t="shared" si="0"/>
-        <v>35, subsection, 2, Luftwechsel, ,</v>
+        <v>35, subsection, 2, {Luftwechsel}, a,</v>
       </c>
     </row>
     <row r="33" spans="2:6" x14ac:dyDescent="0.25">
@@ -898,7 +897,7 @@
       </c>
       <c r="F33" t="str">
         <f t="shared" si="0"/>
-        <v>35, subsection, 2, Nutzungszeiten, ,</v>
+        <v>35, subsection, 2, {Nutzungszeiten}, a,</v>
       </c>
     </row>
     <row r="34" spans="2:6" x14ac:dyDescent="0.25">
@@ -910,7 +909,7 @@
       </c>
       <c r="F34" t="str">
         <f t="shared" si="0"/>
-        <v>35, subsection, 2, Heizung, ,</v>
+        <v>35, subsection, 2, {Heizung}, a,</v>
       </c>
     </row>
     <row r="35" spans="2:6" x14ac:dyDescent="0.25">
@@ -922,7 +921,7 @@
       </c>
       <c r="F35" t="str">
         <f t="shared" si="0"/>
-        <v>36, subsection, 2, Beleuchtung, ,</v>
+        <v>36, subsection, 2, {Beleuchtung}, a,</v>
       </c>
     </row>
     <row r="36" spans="2:6" x14ac:dyDescent="0.25">
@@ -934,7 +933,7 @@
       </c>
       <c r="F36" t="str">
         <f t="shared" si="0"/>
-        <v>36, subsection, 2, Wärmequellen, ,</v>
+        <v>36, subsection, 2, {Wärmequellen}, a,</v>
       </c>
     </row>
     <row r="37" spans="2:6" x14ac:dyDescent="0.25">
@@ -946,7 +945,7 @@
       </c>
       <c r="F37" t="str">
         <f t="shared" si="0"/>
-        <v>40, subsection, 2, Berechnung / Ergebnisse, ,</v>
+        <v>40, subsection, 2, {Berechnung / Ergebnisse}, a,</v>
       </c>
     </row>
     <row r="38" spans="2:6" x14ac:dyDescent="0.25">
@@ -958,7 +957,7 @@
       </c>
       <c r="F38" t="str">
         <f t="shared" si="0"/>
-        <v>43, section, 1, Zone Technik, ,</v>
+        <v>43, section, 1, {Zone Technik}, a,</v>
       </c>
     </row>
     <row r="39" spans="2:6" x14ac:dyDescent="0.25">
@@ -970,7 +969,7 @@
       </c>
       <c r="F39" t="str">
         <f t="shared" si="0"/>
-        <v>43, subsection, 2, Geometrie, ,</v>
+        <v>43, subsection, 2, {Geometrie}, a,</v>
       </c>
     </row>
     <row r="40" spans="2:6" x14ac:dyDescent="0.25">
@@ -982,7 +981,7 @@
       </c>
       <c r="F40" t="str">
         <f t="shared" si="0"/>
-        <v>43, subsection, 2, Hüllfläche, ,</v>
+        <v>43, subsection, 2, {Hüllfläche}, a,</v>
       </c>
     </row>
     <row r="41" spans="2:6" x14ac:dyDescent="0.25">
@@ -994,7 +993,7 @@
       </c>
       <c r="F41" t="str">
         <f t="shared" si="0"/>
-        <v>44, subsection, 2, Raumliste, ,</v>
+        <v>44, subsection, 2, {Raumliste}, a,</v>
       </c>
     </row>
     <row r="42" spans="2:6" x14ac:dyDescent="0.25">
@@ -1006,7 +1005,7 @@
       </c>
       <c r="F42" t="str">
         <f t="shared" si="0"/>
-        <v>44, subsection, 2, Randbedingungen, ,</v>
+        <v>44, subsection, 2, {Randbedingungen}, a,</v>
       </c>
     </row>
     <row r="43" spans="2:6" x14ac:dyDescent="0.25">
@@ -1018,7 +1017,7 @@
       </c>
       <c r="F43" t="str">
         <f t="shared" si="0"/>
-        <v>44, subsection, 2, Luftwechsel, ,</v>
+        <v>44, subsection, 2, {Luftwechsel}, a,</v>
       </c>
     </row>
     <row r="44" spans="2:6" x14ac:dyDescent="0.25">
@@ -1030,7 +1029,7 @@
       </c>
       <c r="F44" t="str">
         <f t="shared" si="0"/>
-        <v>44, subsection, 2, Nutzungszeiten, ,</v>
+        <v>44, subsection, 2, {Nutzungszeiten}, a,</v>
       </c>
     </row>
     <row r="45" spans="2:6" x14ac:dyDescent="0.25">
@@ -1042,7 +1041,7 @@
       </c>
       <c r="F45" t="str">
         <f t="shared" si="0"/>
-        <v>44, subsection, 2, Heizung, ,</v>
+        <v>44, subsection, 2, {Heizung}, a,</v>
       </c>
     </row>
     <row r="46" spans="2:6" x14ac:dyDescent="0.25">
@@ -1054,7 +1053,7 @@
       </c>
       <c r="F46" t="str">
         <f t="shared" si="0"/>
-        <v>45, subsection, 2, Beleuchtung, ,</v>
+        <v>45, subsection, 2, {Beleuchtung}, a,</v>
       </c>
     </row>
     <row r="47" spans="2:6" x14ac:dyDescent="0.25">
@@ -1066,7 +1065,7 @@
       </c>
       <c r="F47" t="str">
         <f t="shared" si="0"/>
-        <v>45, subsection, 2, Wärmequellen, ,</v>
+        <v>45, subsection, 2, {Wärmequellen}, a,</v>
       </c>
     </row>
     <row r="48" spans="2:6" x14ac:dyDescent="0.25">
@@ -1078,7 +1077,7 @@
       </c>
       <c r="F48" t="str">
         <f t="shared" si="0"/>
-        <v>49, subsection, 2, Berechnung / Ergebnisse, ,</v>
+        <v>49, subsection, 2, {Berechnung / Ergebnisse}, a,</v>
       </c>
     </row>
     <row r="49" spans="2:6" x14ac:dyDescent="0.25">
@@ -1090,7 +1089,7 @@
       </c>
       <c r="F49" t="str">
         <f t="shared" si="0"/>
-        <v>52, section, 1, Zone Aufenthaltsraum, ,</v>
+        <v>52, section, 1, {Zone Aufenthaltsraum}, a,</v>
       </c>
     </row>
     <row r="50" spans="2:6" x14ac:dyDescent="0.25">
@@ -1102,7 +1101,7 @@
       </c>
       <c r="F50" t="str">
         <f t="shared" si="0"/>
-        <v>52, subsection, 2, Geometrie, ,</v>
+        <v>52, subsection, 2, {Geometrie}, a,</v>
       </c>
     </row>
     <row r="51" spans="2:6" x14ac:dyDescent="0.25">
@@ -1114,7 +1113,7 @@
       </c>
       <c r="F51" t="str">
         <f t="shared" si="0"/>
-        <v>52, subsection, 2, Hüllfläche, ,</v>
+        <v>52, subsection, 2, {Hüllfläche}, a,</v>
       </c>
     </row>
     <row r="52" spans="2:6" x14ac:dyDescent="0.25">
@@ -1126,7 +1125,7 @@
       </c>
       <c r="F52" t="str">
         <f t="shared" si="0"/>
-        <v>53, subsection, 2, Raumliste, ,</v>
+        <v>53, subsection, 2, {Raumliste}, a,</v>
       </c>
     </row>
     <row r="53" spans="2:6" x14ac:dyDescent="0.25">
@@ -1138,7 +1137,7 @@
       </c>
       <c r="F53" t="str">
         <f t="shared" si="0"/>
-        <v>53, subsection, 2, Randbedingungen, ,</v>
+        <v>53, subsection, 2, {Randbedingungen}, a,</v>
       </c>
     </row>
     <row r="54" spans="2:6" x14ac:dyDescent="0.25">
@@ -1150,7 +1149,7 @@
       </c>
       <c r="F54" t="str">
         <f t="shared" si="0"/>
-        <v>53, subsection, 2, Luftwechsel, ,</v>
+        <v>53, subsection, 2, {Luftwechsel}, a,</v>
       </c>
     </row>
     <row r="55" spans="2:6" x14ac:dyDescent="0.25">
@@ -1162,7 +1161,7 @@
       </c>
       <c r="F55" t="str">
         <f t="shared" si="0"/>
-        <v>53, subsection, 2, Nutzungszeiten, ,</v>
+        <v>53, subsection, 2, {Nutzungszeiten}, a,</v>
       </c>
     </row>
     <row r="56" spans="2:6" x14ac:dyDescent="0.25">
@@ -1174,7 +1173,7 @@
       </c>
       <c r="F56" t="str">
         <f t="shared" si="0"/>
-        <v>53, subsection, 2, Heizung, ,</v>
+        <v>53, subsection, 2, {Heizung}, a,</v>
       </c>
     </row>
     <row r="57" spans="2:6" x14ac:dyDescent="0.25">
@@ -1186,7 +1185,7 @@
       </c>
       <c r="F57" t="str">
         <f t="shared" si="0"/>
-        <v>54, subsection, 2, Kühlung, ,</v>
+        <v>54, subsection, 2, {Kühlung}, a,</v>
       </c>
     </row>
     <row r="58" spans="2:6" x14ac:dyDescent="0.25">
@@ -1198,7 +1197,7 @@
       </c>
       <c r="F58" t="str">
         <f t="shared" si="0"/>
-        <v>54, subsection, 2, Beleuchtung, ,</v>
+        <v>54, subsection, 2, {Beleuchtung}, a,</v>
       </c>
     </row>
     <row r="59" spans="2:6" x14ac:dyDescent="0.25">
@@ -1210,7 +1209,7 @@
       </c>
       <c r="F59" t="str">
         <f t="shared" si="0"/>
-        <v>54, subsection, 2, Wärmequellen, ,</v>
+        <v>54, subsection, 2, {Wärmequellen}, a,</v>
       </c>
     </row>
     <row r="60" spans="2:6" x14ac:dyDescent="0.25">
@@ -1222,7 +1221,7 @@
       </c>
       <c r="F60" t="str">
         <f t="shared" si="0"/>
-        <v>61, subsection, 2, Berechnung / Ergebnisse, ,</v>
+        <v>61, subsection, 2, {Berechnung / Ergebnisse}, a,</v>
       </c>
     </row>
     <row r="61" spans="2:6" x14ac:dyDescent="0.25">
@@ -1234,7 +1233,7 @@
       </c>
       <c r="F61" t="str">
         <f t="shared" si="0"/>
-        <v>64, section, 1, Zone Pfandgutlager, ,</v>
+        <v>64, section, 1, {Zone Pfandgutlager}, a,</v>
       </c>
     </row>
     <row r="62" spans="2:6" x14ac:dyDescent="0.25">
@@ -1246,7 +1245,7 @@
       </c>
       <c r="F62" t="str">
         <f t="shared" si="0"/>
-        <v>64, subsection, 2, Geometrie, ,</v>
+        <v>64, subsection, 2, {Geometrie}, a,</v>
       </c>
     </row>
     <row r="63" spans="2:6" x14ac:dyDescent="0.25">
@@ -1258,7 +1257,7 @@
       </c>
       <c r="F63" t="str">
         <f t="shared" si="0"/>
-        <v>64, subsection, 2, Hüllfläche, ,</v>
+        <v>64, subsection, 2, {Hüllfläche}, a,</v>
       </c>
     </row>
     <row r="64" spans="2:6" x14ac:dyDescent="0.25">
@@ -1270,7 +1269,7 @@
       </c>
       <c r="F64" t="str">
         <f t="shared" si="0"/>
-        <v>65, subsection, 2, Raumliste, ,</v>
+        <v>65, subsection, 2, {Raumliste}, a,</v>
       </c>
     </row>
     <row r="65" spans="2:6" x14ac:dyDescent="0.25">
@@ -1282,7 +1281,7 @@
       </c>
       <c r="F65" t="str">
         <f t="shared" si="0"/>
-        <v>65, subsection, 2, Randbedingungen, ,</v>
+        <v>65, subsection, 2, {Randbedingungen}, a,</v>
       </c>
     </row>
     <row r="66" spans="2:6" x14ac:dyDescent="0.25">
@@ -1294,7 +1293,7 @@
       </c>
       <c r="F66" t="str">
         <f t="shared" si="0"/>
-        <v>65, subsection, 2, Luftwechsel, ,</v>
+        <v>65, subsection, 2, {Luftwechsel}, a,</v>
       </c>
     </row>
     <row r="67" spans="2:6" x14ac:dyDescent="0.25">
@@ -1306,7 +1305,7 @@
       </c>
       <c r="F67" t="str">
         <f t="shared" si="0"/>
-        <v>65, subsection, 2, Nutzungszeiten, ,</v>
+        <v>65, subsection, 2, {Nutzungszeiten}, a,</v>
       </c>
     </row>
     <row r="68" spans="2:6" x14ac:dyDescent="0.25">
@@ -1317,8 +1316,8 @@
         <v>65</v>
       </c>
       <c r="F68" t="str">
-        <f t="shared" ref="F68:F131" si="1">CONCATENATE(D68,", ",IF(ISBLANK(A68)=FALSE,A$3,IF(ISBLANK(B68)=FALSE,B$3,C$3)),", ",IF(ISBLANK(A68)=FALSE,0,IF(ISBLANK(B68)=FALSE,1,2)),", ",IF(ISBLANK(A68)=FALSE,A68,IF(ISBLANK(B68)=FALSE,B68,C68)),IF(ISBLANK(D69)=TRUE,",",", ,"))</f>
-        <v>65, subsection, 2, Heizung, ,</v>
+        <f t="shared" si="0"/>
+        <v>65, subsection, 2, {Heizung}, a,</v>
       </c>
     </row>
     <row r="69" spans="2:6" x14ac:dyDescent="0.25">
@@ -1329,8 +1328,8 @@
         <v>66</v>
       </c>
       <c r="F69" t="str">
-        <f t="shared" si="1"/>
-        <v>66, subsection, 2, Lüftung, ,</v>
+        <f t="shared" ref="F69:F132" si="1">CONCATENATE(D69,", ",IF(ISBLANK(A69)=FALSE,A$3,IF(ISBLANK(B69)=FALSE,B$3,C$3)),", ",IF(ISBLANK(A69)=FALSE,0,IF(ISBLANK(B69)=FALSE,1,2)),", {",IF(ISBLANK(A69)=FALSE,A69,IF(ISBLANK(B69)=FALSE,B69,C69)),"}, a",IF(ISBLANK(D70)=TRUE,"",","))</f>
+        <v>66, subsection, 2, {Lüftung}, a,</v>
       </c>
     </row>
     <row r="70" spans="2:6" x14ac:dyDescent="0.25">
@@ -1342,7 +1341,7 @@
       </c>
       <c r="F70" t="str">
         <f t="shared" si="1"/>
-        <v>66, subsection, 2, Beleuchtung, ,</v>
+        <v>66, subsection, 2, {Beleuchtung}, a,</v>
       </c>
     </row>
     <row r="71" spans="2:6" x14ac:dyDescent="0.25">
@@ -1354,7 +1353,7 @@
       </c>
       <c r="F71" t="str">
         <f t="shared" si="1"/>
-        <v>66, subsection, 2, Wärmequellen, ,</v>
+        <v>66, subsection, 2, {Wärmequellen}, a,</v>
       </c>
     </row>
     <row r="72" spans="2:6" x14ac:dyDescent="0.25">
@@ -1366,7 +1365,7 @@
       </c>
       <c r="F72" t="str">
         <f t="shared" si="1"/>
-        <v>66, subsection, 2, Gezielter Luftaustausch mit Zone Pfangutlager, ,</v>
+        <v>66, subsection, 2, {Gezielter Luftaustausch mit Zone Pfangutlager}, a,</v>
       </c>
     </row>
     <row r="73" spans="2:6" x14ac:dyDescent="0.25">
@@ -1378,7 +1377,7 @@
       </c>
       <c r="F73" t="str">
         <f t="shared" si="1"/>
-        <v>66, subsection, 2, Konfiguration Lüftungsanlage, ,</v>
+        <v>66, subsection, 2, {Konfiguration Lüftungsanlage}, a,</v>
       </c>
     </row>
     <row r="74" spans="2:6" x14ac:dyDescent="0.25">
@@ -1390,7 +1389,7 @@
       </c>
       <c r="F74" t="str">
         <f t="shared" si="1"/>
-        <v>70, subsection, 2, Berechnung / Ergebnisse, ,</v>
+        <v>70, subsection, 2, {Berechnung / Ergebnisse}, a,</v>
       </c>
     </row>
     <row r="75" spans="2:6" x14ac:dyDescent="0.25">
@@ -1402,7 +1401,7 @@
       </c>
       <c r="F75" t="str">
         <f t="shared" si="1"/>
-        <v>73, section, 1, Zone Aktenraum, ,</v>
+        <v>73, section, 1, {Zone Aktenraum}, a,</v>
       </c>
     </row>
     <row r="76" spans="2:6" x14ac:dyDescent="0.25">
@@ -1414,7 +1413,7 @@
       </c>
       <c r="F76" t="str">
         <f t="shared" si="1"/>
-        <v>73, subsection, 2, Geometrie, ,</v>
+        <v>73, subsection, 2, {Geometrie}, a,</v>
       </c>
     </row>
     <row r="77" spans="2:6" x14ac:dyDescent="0.25">
@@ -1426,7 +1425,7 @@
       </c>
       <c r="F77" t="str">
         <f t="shared" si="1"/>
-        <v>73, subsection, 2, Hüllfläche, ,</v>
+        <v>73, subsection, 2, {Hüllfläche}, a,</v>
       </c>
     </row>
     <row r="78" spans="2:6" x14ac:dyDescent="0.25">
@@ -1438,7 +1437,7 @@
       </c>
       <c r="F78" t="str">
         <f t="shared" si="1"/>
-        <v>74, subsection, 2, Raumliste, ,</v>
+        <v>74, subsection, 2, {Raumliste}, a,</v>
       </c>
     </row>
     <row r="79" spans="2:6" x14ac:dyDescent="0.25">
@@ -1450,7 +1449,7 @@
       </c>
       <c r="F79" t="str">
         <f t="shared" si="1"/>
-        <v>74, subsection, 2, Randbedingungen, ,</v>
+        <v>74, subsection, 2, {Randbedingungen}, a,</v>
       </c>
     </row>
     <row r="80" spans="2:6" x14ac:dyDescent="0.25">
@@ -1462,7 +1461,7 @@
       </c>
       <c r="F80" t="str">
         <f t="shared" si="1"/>
-        <v>74, subsection, 2, Luftwechsel, ,</v>
+        <v>74, subsection, 2, {Luftwechsel}, a,</v>
       </c>
     </row>
     <row r="81" spans="2:6" x14ac:dyDescent="0.25">
@@ -1474,7 +1473,7 @@
       </c>
       <c r="F81" t="str">
         <f t="shared" si="1"/>
-        <v>74, subsection, 2, Nutzungszeiten, ,</v>
+        <v>74, subsection, 2, {Nutzungszeiten}, a,</v>
       </c>
     </row>
     <row r="82" spans="2:6" x14ac:dyDescent="0.25">
@@ -1486,7 +1485,7 @@
       </c>
       <c r="F82" t="str">
         <f t="shared" si="1"/>
-        <v>74, subsection, 2, Heizung, ,</v>
+        <v>74, subsection, 2, {Heizung}, a,</v>
       </c>
     </row>
     <row r="83" spans="2:6" x14ac:dyDescent="0.25">
@@ -1498,7 +1497,7 @@
       </c>
       <c r="F83" t="str">
         <f t="shared" si="1"/>
-        <v>75, subsection, 2, Kühlung, ,</v>
+        <v>75, subsection, 2, {Kühlung}, a,</v>
       </c>
     </row>
     <row r="84" spans="2:6" x14ac:dyDescent="0.25">
@@ -1510,7 +1509,7 @@
       </c>
       <c r="F84" t="str">
         <f t="shared" si="1"/>
-        <v>75, subsection, 2, Lüftung, ,</v>
+        <v>75, subsection, 2, {Lüftung}, a,</v>
       </c>
     </row>
     <row r="85" spans="2:6" x14ac:dyDescent="0.25">
@@ -1522,7 +1521,7 @@
       </c>
       <c r="F85" t="str">
         <f t="shared" si="1"/>
-        <v>75, subsection, 2, Beleuchtung, ,</v>
+        <v>75, subsection, 2, {Beleuchtung}, a,</v>
       </c>
     </row>
     <row r="86" spans="2:6" x14ac:dyDescent="0.25">
@@ -1534,7 +1533,7 @@
       </c>
       <c r="F86" t="str">
         <f t="shared" si="1"/>
-        <v>75, subsection, 2, Wärmequellen, ,</v>
+        <v>75, subsection, 2, {Wärmequellen}, a,</v>
       </c>
     </row>
     <row r="87" spans="2:6" x14ac:dyDescent="0.25">
@@ -1546,7 +1545,7 @@
       </c>
       <c r="F87" t="str">
         <f t="shared" si="1"/>
-        <v>75, subsection, 2, Konfiguration Lüftungsanlage, ,</v>
+        <v>75, subsection, 2, {Konfiguration Lüftungsanlage}, a,</v>
       </c>
     </row>
     <row r="88" spans="2:6" x14ac:dyDescent="0.25">
@@ -1558,7 +1557,7 @@
       </c>
       <c r="F88" t="str">
         <f t="shared" si="1"/>
-        <v>83, subsection, 2, Berechnung / Ergebnisse, ,</v>
+        <v>83, subsection, 2, {Berechnung / Ergebnisse}, a,</v>
       </c>
     </row>
     <row r="89" spans="2:6" x14ac:dyDescent="0.25">
@@ -1570,7 +1569,7 @@
       </c>
       <c r="F89" t="str">
         <f t="shared" si="1"/>
-        <v>86, section, 1, Zone WC, Umkleide, ,</v>
+        <v>86, section, 1, {Zone WC, Umkleide}, a,</v>
       </c>
     </row>
     <row r="90" spans="2:6" x14ac:dyDescent="0.25">
@@ -1582,7 +1581,7 @@
       </c>
       <c r="F90" t="str">
         <f t="shared" si="1"/>
-        <v>86, subsection, 2, Geometrie, ,</v>
+        <v>86, subsection, 2, {Geometrie}, a,</v>
       </c>
     </row>
     <row r="91" spans="2:6" x14ac:dyDescent="0.25">
@@ -1594,7 +1593,7 @@
       </c>
       <c r="F91" t="str">
         <f t="shared" si="1"/>
-        <v>86, subsection, 2, Hüllfläche, ,</v>
+        <v>86, subsection, 2, {Hüllfläche}, a,</v>
       </c>
     </row>
     <row r="92" spans="2:6" x14ac:dyDescent="0.25">
@@ -1606,7 +1605,7 @@
       </c>
       <c r="F92" t="str">
         <f t="shared" si="1"/>
-        <v>87, subsection, 2, Raumliste, ,</v>
+        <v>87, subsection, 2, {Raumliste}, a,</v>
       </c>
     </row>
     <row r="93" spans="2:6" x14ac:dyDescent="0.25">
@@ -1618,7 +1617,7 @@
       </c>
       <c r="F93" t="str">
         <f t="shared" si="1"/>
-        <v>87, subsection, 2, Randbedingungen, ,</v>
+        <v>87, subsection, 2, {Randbedingungen}, a,</v>
       </c>
     </row>
     <row r="94" spans="2:6" x14ac:dyDescent="0.25">
@@ -1630,7 +1629,7 @@
       </c>
       <c r="F94" t="str">
         <f t="shared" si="1"/>
-        <v>87, subsection, 2, Luftwechsel, ,</v>
+        <v>87, subsection, 2, {Luftwechsel}, a,</v>
       </c>
     </row>
     <row r="95" spans="2:6" x14ac:dyDescent="0.25">
@@ -1642,7 +1641,7 @@
       </c>
       <c r="F95" t="str">
         <f t="shared" si="1"/>
-        <v>87, subsection, 2, Nutzungszeiten, ,</v>
+        <v>87, subsection, 2, {Nutzungszeiten}, a,</v>
       </c>
     </row>
     <row r="96" spans="2:6" x14ac:dyDescent="0.25">
@@ -1654,7 +1653,7 @@
       </c>
       <c r="F96" t="str">
         <f t="shared" si="1"/>
-        <v>88, subsection, 2, Heizung, ,</v>
+        <v>88, subsection, 2, {Heizung}, a,</v>
       </c>
     </row>
     <row r="97" spans="2:6" x14ac:dyDescent="0.25">
@@ -1666,7 +1665,7 @@
       </c>
       <c r="F97" t="str">
         <f t="shared" si="1"/>
-        <v>88, subsection, 2, Lüftung, ,</v>
+        <v>88, subsection, 2, {Lüftung}, a,</v>
       </c>
     </row>
     <row r="98" spans="2:6" x14ac:dyDescent="0.25">
@@ -1678,7 +1677,7 @@
       </c>
       <c r="F98" t="str">
         <f t="shared" si="1"/>
-        <v>88, subsection, 2, Beleuchtung, ,</v>
+        <v>88, subsection, 2, {Beleuchtung}, a,</v>
       </c>
     </row>
     <row r="99" spans="2:6" x14ac:dyDescent="0.25">
@@ -1690,7 +1689,7 @@
       </c>
       <c r="F99" t="str">
         <f t="shared" si="1"/>
-        <v>88, subsection, 2, Wärmequellen, ,</v>
+        <v>88, subsection, 2, {Wärmequellen}, a,</v>
       </c>
     </row>
     <row r="100" spans="2:6" x14ac:dyDescent="0.25">
@@ -1702,7 +1701,7 @@
       </c>
       <c r="F100" t="str">
         <f t="shared" si="1"/>
-        <v>88, subsection, 2, Konfiguration Lüftungsanlage, ,</v>
+        <v>88, subsection, 2, {Konfiguration Lüftungsanlage}, a,</v>
       </c>
     </row>
     <row r="101" spans="2:6" x14ac:dyDescent="0.25">
@@ -1714,7 +1713,7 @@
       </c>
       <c r="F101" t="str">
         <f t="shared" si="1"/>
-        <v>93, subsection, 2, Berechnung / Ergebnisse, ,</v>
+        <v>93, subsection, 2, {Berechnung / Ergebnisse}, a,</v>
       </c>
     </row>
     <row r="102" spans="2:6" x14ac:dyDescent="0.25">
@@ -1726,7 +1725,7 @@
       </c>
       <c r="F102" t="str">
         <f t="shared" si="1"/>
-        <v>96, section, 1, Zone RVL Büro, ,</v>
+        <v>96, section, 1, {Zone RVL Büro}, a,</v>
       </c>
     </row>
     <row r="103" spans="2:6" x14ac:dyDescent="0.25">
@@ -1738,7 +1737,7 @@
       </c>
       <c r="F103" t="str">
         <f t="shared" si="1"/>
-        <v>96, subsection, 2, Geometrie, ,</v>
+        <v>96, subsection, 2, {Geometrie}, a,</v>
       </c>
     </row>
     <row r="104" spans="2:6" x14ac:dyDescent="0.25">
@@ -1750,7 +1749,7 @@
       </c>
       <c r="F104" t="str">
         <f t="shared" si="1"/>
-        <v>96, subsection, 2, Hüllfläche, ,</v>
+        <v>96, subsection, 2, {Hüllfläche}, a,</v>
       </c>
     </row>
     <row r="105" spans="2:6" x14ac:dyDescent="0.25">
@@ -1762,7 +1761,7 @@
       </c>
       <c r="F105" t="str">
         <f t="shared" si="1"/>
-        <v>97, subsection, 2, Raumliste, ,</v>
+        <v>97, subsection, 2, {Raumliste}, a,</v>
       </c>
     </row>
     <row r="106" spans="2:6" x14ac:dyDescent="0.25">
@@ -1774,7 +1773,7 @@
       </c>
       <c r="F106" t="str">
         <f t="shared" si="1"/>
-        <v>97, subsection, 2, Randbedingungen, ,</v>
+        <v>97, subsection, 2, {Randbedingungen}, a,</v>
       </c>
     </row>
     <row r="107" spans="2:6" x14ac:dyDescent="0.25">
@@ -1786,7 +1785,7 @@
       </c>
       <c r="F107" t="str">
         <f t="shared" si="1"/>
-        <v>97, subsection, 2, Luftwechsel, ,</v>
+        <v>97, subsection, 2, {Luftwechsel}, a,</v>
       </c>
     </row>
     <row r="108" spans="2:6" x14ac:dyDescent="0.25">
@@ -1798,7 +1797,7 @@
       </c>
       <c r="F108" t="str">
         <f t="shared" si="1"/>
-        <v>97, subsection, 2, Nutzungszeiten, ,</v>
+        <v>97, subsection, 2, {Nutzungszeiten}, a,</v>
       </c>
     </row>
     <row r="109" spans="2:6" x14ac:dyDescent="0.25">
@@ -1810,7 +1809,7 @@
       </c>
       <c r="F109" t="str">
         <f t="shared" si="1"/>
-        <v>97, subsection, 2, Heizung, ,</v>
+        <v>97, subsection, 2, {Heizung}, a,</v>
       </c>
     </row>
     <row r="110" spans="2:6" x14ac:dyDescent="0.25">
@@ -1822,7 +1821,7 @@
       </c>
       <c r="F110" t="str">
         <f t="shared" si="1"/>
-        <v>98, subsection, 2, Kühlung, ,</v>
+        <v>98, subsection, 2, {Kühlung}, a,</v>
       </c>
     </row>
     <row r="111" spans="2:6" x14ac:dyDescent="0.25">
@@ -1834,7 +1833,7 @@
       </c>
       <c r="F111" t="str">
         <f t="shared" si="1"/>
-        <v>98, subsection, 2, Beleuchtung, ,</v>
+        <v>98, subsection, 2, {Beleuchtung}, a,</v>
       </c>
     </row>
     <row r="112" spans="2:6" x14ac:dyDescent="0.25">
@@ -1846,7 +1845,7 @@
       </c>
       <c r="F112" t="str">
         <f t="shared" si="1"/>
-        <v>98, subsection, 2, Wärmequellen, ,</v>
+        <v>98, subsection, 2, {Wärmequellen}, a,</v>
       </c>
     </row>
     <row r="113" spans="2:6" x14ac:dyDescent="0.25">
@@ -1858,7 +1857,7 @@
       </c>
       <c r="F113" t="str">
         <f t="shared" si="1"/>
-        <v>105, subsection, 2, Berechnung / Ergebnisse, ,</v>
+        <v>105, subsection, 2, {Berechnung / Ergebnisse}, a,</v>
       </c>
     </row>
     <row r="114" spans="2:6" x14ac:dyDescent="0.25">
@@ -1870,7 +1869,7 @@
       </c>
       <c r="F114" t="str">
         <f t="shared" si="1"/>
-        <v>108, section, 1, Zone Dachraum, ,</v>
+        <v>108, section, 1, {Zone Dachraum}, a,</v>
       </c>
     </row>
     <row r="115" spans="2:6" x14ac:dyDescent="0.25">
@@ -1882,7 +1881,7 @@
       </c>
       <c r="F115" t="str">
         <f t="shared" si="1"/>
-        <v>108, subsection, 2, Geometrie, ,</v>
+        <v>108, subsection, 2, {Geometrie}, a,</v>
       </c>
     </row>
     <row r="116" spans="2:6" x14ac:dyDescent="0.25">
@@ -1894,7 +1893,7 @@
       </c>
       <c r="F116" t="str">
         <f t="shared" si="1"/>
-        <v>109, subsection, 2, Raumliste, ,</v>
+        <v>109, subsection, 2, {Raumliste}, a,</v>
       </c>
     </row>
     <row r="117" spans="2:6" x14ac:dyDescent="0.25">
@@ -1906,7 +1905,7 @@
       </c>
       <c r="F117" t="str">
         <f t="shared" si="1"/>
-        <v>109, subsection, 2, Randbedingungen, ,</v>
+        <v>109, subsection, 2, {Randbedingungen}, a,</v>
       </c>
     </row>
     <row r="118" spans="2:6" x14ac:dyDescent="0.25">
@@ -1918,7 +1917,7 @@
       </c>
       <c r="F118" t="str">
         <f t="shared" si="1"/>
-        <v>109, subsection, 2, Luftwechsel, ,</v>
+        <v>109, subsection, 2, {Luftwechsel}, a,</v>
       </c>
     </row>
     <row r="119" spans="2:6" x14ac:dyDescent="0.25">
@@ -1930,7 +1929,7 @@
       </c>
       <c r="F119" t="str">
         <f t="shared" si="1"/>
-        <v>109, subsection, 2, Nutzungszeiten, ,</v>
+        <v>109, subsection, 2, {Nutzungszeiten}, a,</v>
       </c>
     </row>
     <row r="120" spans="2:6" x14ac:dyDescent="0.25">
@@ -1942,7 +1941,7 @@
       </c>
       <c r="F120" t="str">
         <f t="shared" si="1"/>
-        <v>109, subsection, 2, Beleuchtung, ,</v>
+        <v>109, subsection, 2, {Beleuchtung}, a,</v>
       </c>
     </row>
     <row r="121" spans="2:6" x14ac:dyDescent="0.25">
@@ -1954,7 +1953,7 @@
       </c>
       <c r="F121" t="str">
         <f t="shared" si="1"/>
-        <v>110, subsection, 2, Wärmequellen, ,</v>
+        <v>110, subsection, 2, {Wärmequellen}, a,</v>
       </c>
     </row>
     <row r="122" spans="2:6" x14ac:dyDescent="0.25">
@@ -1966,7 +1965,7 @@
       </c>
       <c r="F122" t="str">
         <f t="shared" si="1"/>
-        <v>111, subsection, 2, Berechnung / Ergebnisse, ,</v>
+        <v>111, subsection, 2, {Berechnung / Ergebnisse}, a,</v>
       </c>
     </row>
     <row r="123" spans="2:6" x14ac:dyDescent="0.25">
@@ -1978,7 +1977,7 @@
       </c>
       <c r="F123" t="str">
         <f t="shared" si="1"/>
-        <v>113, section, 1, Anlagentechnik, ,</v>
+        <v>113, section, 1, {Anlagentechnik}, a,</v>
       </c>
     </row>
     <row r="124" spans="2:6" x14ac:dyDescent="0.25">
@@ -1990,7 +1989,7 @@
       </c>
       <c r="F124" t="str">
         <f t="shared" si="1"/>
-        <v>113, subsection, 2, Heizungsanlage, ,</v>
+        <v>113, subsection, 2, {Heizungsanlage}, a,</v>
       </c>
     </row>
     <row r="125" spans="2:6" x14ac:dyDescent="0.25">
@@ -2002,7 +2001,7 @@
       </c>
       <c r="F125" t="str">
         <f t="shared" si="1"/>
-        <v>118, subsection, 2, Trinkwasseranlage, ,</v>
+        <v>118, subsection, 2, {Trinkwasseranlage}, a,</v>
       </c>
     </row>
     <row r="126" spans="2:6" x14ac:dyDescent="0.25">
@@ -2014,7 +2013,7 @@
       </c>
       <c r="F126" t="str">
         <f t="shared" si="1"/>
-        <v>119, subsection, 2, Kühlungsanlage, ,</v>
+        <v>119, subsection, 2, {Kühlungsanlage}, a,</v>
       </c>
     </row>
     <row r="127" spans="2:6" x14ac:dyDescent="0.25">
@@ -2026,7 +2025,7 @@
       </c>
       <c r="F127" t="str">
         <f t="shared" si="1"/>
-        <v>123, subsection, 2, RLT-Anlage, ,</v>
+        <v>123, subsection, 2, {RLT-Anlage}, a,</v>
       </c>
     </row>
     <row r="128" spans="2:6" x14ac:dyDescent="0.25">
@@ -2038,7 +2037,7 @@
       </c>
       <c r="F128" t="str">
         <f t="shared" si="1"/>
-        <v>127, subsection, 2, Photovoltaikanlage, ,</v>
+        <v>127, subsection, 2, {Photovoltaikanlage}, a,</v>
       </c>
     </row>
     <row r="129" spans="2:6" x14ac:dyDescent="0.25">
@@ -2050,7 +2049,7 @@
       </c>
       <c r="F129" t="str">
         <f t="shared" si="1"/>
-        <v>128, section, 1, Beleuchtung, ,</v>
+        <v>128, section, 1, {Beleuchtung}, a,</v>
       </c>
     </row>
     <row r="130" spans="2:6" x14ac:dyDescent="0.25">
@@ -2062,7 +2061,7 @@
       </c>
       <c r="F130" t="str">
         <f t="shared" si="1"/>
-        <v>128, subsection, 2, Verkaufsraum, ,</v>
+        <v>128, subsection, 2, {Verkaufsraum}, a,</v>
       </c>
     </row>
     <row r="131" spans="2:6" x14ac:dyDescent="0.25">
@@ -2074,7 +2073,7 @@
       </c>
       <c r="F131" t="str">
         <f t="shared" si="1"/>
-        <v>128, subsection, 2, Lager, ,</v>
+        <v>128, subsection, 2, {Lager}, a,</v>
       </c>
     </row>
     <row r="132" spans="2:6" x14ac:dyDescent="0.25">
@@ -2085,8 +2084,8 @@
         <v>128</v>
       </c>
       <c r="F132" t="str">
-        <f t="shared" ref="F132:F141" si="2">CONCATENATE(D132,", ",IF(ISBLANK(A132)=FALSE,A$3,IF(ISBLANK(B132)=FALSE,B$3,C$3)),", ",IF(ISBLANK(A132)=FALSE,0,IF(ISBLANK(B132)=FALSE,1,2)),", ",IF(ISBLANK(A132)=FALSE,A132,IF(ISBLANK(B132)=FALSE,B132,C132)),IF(ISBLANK(D133)=TRUE,",",", ,"))</f>
-        <v>128, subsection, 2, Technik, ,</v>
+        <f t="shared" si="1"/>
+        <v>128, subsection, 2, {Technik}, a,</v>
       </c>
     </row>
     <row r="133" spans="2:6" x14ac:dyDescent="0.25">
@@ -2097,8 +2096,8 @@
         <v>129</v>
       </c>
       <c r="F133" t="str">
-        <f t="shared" si="2"/>
-        <v>129, subsection, 2, Aufenthaltsraum, ,</v>
+        <f t="shared" ref="F133:F141" si="2">CONCATENATE(D133,", ",IF(ISBLANK(A133)=FALSE,A$3,IF(ISBLANK(B133)=FALSE,B$3,C$3)),", ",IF(ISBLANK(A133)=FALSE,0,IF(ISBLANK(B133)=FALSE,1,2)),", {",IF(ISBLANK(A133)=FALSE,A133,IF(ISBLANK(B133)=FALSE,B133,C133)),"}, a",IF(ISBLANK(D134)=TRUE,"",","))</f>
+        <v>129, subsection, 2, {Aufenthaltsraum}, a,</v>
       </c>
     </row>
     <row r="134" spans="2:6" x14ac:dyDescent="0.25">
@@ -2110,7 +2109,7 @@
       </c>
       <c r="F134" t="str">
         <f t="shared" si="2"/>
-        <v>130, subsection, 2, Pfandgutlager, ,</v>
+        <v>130, subsection, 2, {Pfandgutlager}, a,</v>
       </c>
     </row>
     <row r="135" spans="2:6" x14ac:dyDescent="0.25">
@@ -2122,7 +2121,7 @@
       </c>
       <c r="F135" t="str">
         <f t="shared" si="2"/>
-        <v>130, subsection, 2, Aktenraum, ,</v>
+        <v>130, subsection, 2, {Aktenraum}, a,</v>
       </c>
     </row>
     <row r="136" spans="2:6" x14ac:dyDescent="0.25">
@@ -2134,7 +2133,7 @@
       </c>
       <c r="F136" t="str">
         <f t="shared" si="2"/>
-        <v>131, subsection, 2, WC, Umkleide, ,</v>
+        <v>131, subsection, 2, {WC, Umkleide}, a,</v>
       </c>
     </row>
     <row r="137" spans="2:6" x14ac:dyDescent="0.25">
@@ -2146,7 +2145,7 @@
       </c>
       <c r="F137" t="str">
         <f t="shared" si="2"/>
-        <v>131, subsection, 2, RVL Büro, ,</v>
+        <v>131, subsection, 2, {RVL Büro}, a,</v>
       </c>
     </row>
     <row r="138" spans="2:6" x14ac:dyDescent="0.25">
@@ -2158,7 +2157,7 @@
       </c>
       <c r="F138" t="str">
         <f t="shared" si="2"/>
-        <v>132, subsection, 2, Dachraum, ,</v>
+        <v>132, subsection, 2, {Dachraum}, a,</v>
       </c>
     </row>
     <row r="139" spans="2:6" x14ac:dyDescent="0.25">
@@ -2170,7 +2169,7 @@
       </c>
       <c r="F139" t="str">
         <f t="shared" si="2"/>
-        <v>133, section, 1, Übersicht der verwendeten Normen und Verordnungen, ,</v>
+        <v>133, section, 1, {Übersicht der verwendeten Normen und Verordnungen}, a,</v>
       </c>
     </row>
     <row r="140" spans="2:6" x14ac:dyDescent="0.25">
@@ -2182,7 +2181,7 @@
       </c>
       <c r="F140" t="str">
         <f t="shared" si="2"/>
-        <v>134, section, 1, Brennstoffdaten, ,</v>
+        <v>134, section, 1, {Brennstoffdaten}, a,</v>
       </c>
     </row>
     <row r="141" spans="2:6" x14ac:dyDescent="0.25">
@@ -2194,7 +2193,7 @@
       </c>
       <c r="F141" t="str">
         <f t="shared" si="2"/>
-        <v>134, section, 1, Anhang - U - Wert - Ermittlung,</v>
+        <v>134, section, 1, {Anhang - U - Wert - Ermittlung}, a</v>
       </c>
     </row>
   </sheetData>
@@ -2206,8 +2205,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F129"/>
   <sheetViews>
-    <sheetView topLeftCell="A94" workbookViewId="0">
-      <selection activeCell="I108" sqref="I108"/>
+    <sheetView tabSelected="1" topLeftCell="A94" workbookViewId="0">
+      <selection activeCell="F4" sqref="F4:F129"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2245,8 +2244,8 @@
         <v>2</v>
       </c>
       <c r="F4" t="str">
-        <f>CONCATENATE(D4,", ",IF(ISBLANK(A4)=FALSE,A$3,IF(ISBLANK(B4)=FALSE,B$3,C$3)),", ",IF(ISBLANK(A4)=FALSE,0,IF(ISBLANK(B4)=FALSE,1,2)),", ",IF(ISBLANK(A4)=FALSE,A4,IF(ISBLANK(B4)=FALSE,B4,C4)),IF(ISBLANK(D5)=TRUE,",",", ,"))</f>
-        <v>2, section, 1, Allgemeine Angaben zum Gebäude, ,</v>
+        <f>CONCATENATE(D4,", ",IF(ISBLANK(A4)=FALSE,A$3,IF(ISBLANK(B4)=FALSE,B$3,C$3)),", ",IF(ISBLANK(A4)=FALSE,0,IF(ISBLANK(B4)=FALSE,1,2)),", {",IF(ISBLANK(A4)=FALSE,A4,IF(ISBLANK(B4)=FALSE,B4,C4)),"}, a",IF(ISBLANK(D5)=TRUE,"",","))</f>
+        <v>2, section, 1, {Allgemeine Angaben zum Gebäude}, a,</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
@@ -2257,8 +2256,8 @@
         <v>3</v>
       </c>
       <c r="F5" t="str">
-        <f t="shared" ref="F5:F68" si="0">CONCATENATE(D5,", ",IF(ISBLANK(A5)=FALSE,A$3,IF(ISBLANK(B5)=FALSE,B$3,C$3)),", ",IF(ISBLANK(A5)=FALSE,0,IF(ISBLANK(B5)=FALSE,1,2)),", ",IF(ISBLANK(A5)=FALSE,A5,IF(ISBLANK(B5)=FALSE,B5,C5)),IF(ISBLANK(D6)=TRUE,",",", ,"))</f>
-        <v>3, subsection, 2, Zonen, ,</v>
+        <f t="shared" ref="F5:F68" si="0">CONCATENATE(D5,", ",IF(ISBLANK(A5)=FALSE,A$3,IF(ISBLANK(B5)=FALSE,B$3,C$3)),", ",IF(ISBLANK(A5)=FALSE,0,IF(ISBLANK(B5)=FALSE,1,2)),", {",IF(ISBLANK(A5)=FALSE,A5,IF(ISBLANK(B5)=FALSE,B5,C5)),"}, a",IF(ISBLANK(D6)=TRUE,"",","))</f>
+        <v>3, subsection, 2, {Zonen}, a,</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
@@ -2270,7 +2269,7 @@
       </c>
       <c r="F6" t="str">
         <f t="shared" si="0"/>
-        <v>4, subsection, 2, Bauteilflächen, ,</v>
+        <v>4, subsection, 2, {Bauteilflächen}, a,</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
@@ -2282,7 +2281,7 @@
       </c>
       <c r="F7" t="str">
         <f t="shared" si="0"/>
-        <v>8, subsection, 2, Raumliste, ,</v>
+        <v>8, subsection, 2, {Raumliste}, a,</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
@@ -2294,7 +2293,7 @@
       </c>
       <c r="F8" t="str">
         <f t="shared" si="0"/>
-        <v>9, subsection, 2, Energiebilanz, ,</v>
+        <v>9, subsection, 2, {Energiebilanz}, a,</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
@@ -2306,7 +2305,7 @@
       </c>
       <c r="F9" t="str">
         <f t="shared" si="0"/>
-        <v>15, section, 1, Bewertung des Gebäudes entsprechend den GEG-Anforderungen, ,</v>
+        <v>15, section, 1, {Bewertung des Gebäudes entsprechend den GEG-Anforderungen}, a,</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
@@ -2318,7 +2317,7 @@
       </c>
       <c r="F10" t="str">
         <f t="shared" si="0"/>
-        <v>16, section, 1, Zone Verkaufsraum, ,</v>
+        <v>16, section, 1, {Zone Verkaufsraum}, a,</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
@@ -2330,7 +2329,7 @@
       </c>
       <c r="F11" t="str">
         <f t="shared" si="0"/>
-        <v>16, subsection, 2, Geometrie, ,</v>
+        <v>16, subsection, 2, {Geometrie}, a,</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
@@ -2342,7 +2341,7 @@
       </c>
       <c r="F12" t="str">
         <f t="shared" si="0"/>
-        <v>17, subsection, 2, Raumliste, ,</v>
+        <v>17, subsection, 2, {Raumliste}, a,</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
@@ -2354,7 +2353,7 @@
       </c>
       <c r="F13" t="str">
         <f t="shared" si="0"/>
-        <v>17, subsection, 2, Randbedingungen, ,</v>
+        <v>17, subsection, 2, {Randbedingungen}, a,</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
@@ -2366,7 +2365,7 @@
       </c>
       <c r="F14" t="str">
         <f t="shared" si="0"/>
-        <v>17, subsection, 2, Luftwechsel, ,</v>
+        <v>17, subsection, 2, {Luftwechsel}, a,</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
@@ -2378,7 +2377,7 @@
       </c>
       <c r="F15" t="str">
         <f t="shared" si="0"/>
-        <v>17, subsection, 2, Nutzungszeiten, ,</v>
+        <v>17, subsection, 2, {Nutzungszeiten}, a,</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
@@ -2390,7 +2389,7 @@
       </c>
       <c r="F16" t="str">
         <f t="shared" si="0"/>
-        <v>17, subsection, 2, Heizung, ,</v>
+        <v>17, subsection, 2, {Heizung}, a,</v>
       </c>
     </row>
     <row r="17" spans="2:6" x14ac:dyDescent="0.25">
@@ -2402,7 +2401,7 @@
       </c>
       <c r="F17" t="str">
         <f t="shared" si="0"/>
-        <v>18, subsection, 2, Kühlung, ,</v>
+        <v>18, subsection, 2, {Kühlung}, a,</v>
       </c>
     </row>
     <row r="18" spans="2:6" x14ac:dyDescent="0.25">
@@ -2414,7 +2413,7 @@
       </c>
       <c r="F18" t="str">
         <f t="shared" si="0"/>
-        <v>18, subsection, 2, Lüftung, ,</v>
+        <v>18, subsection, 2, {Lüftung}, a,</v>
       </c>
     </row>
     <row r="19" spans="2:6" x14ac:dyDescent="0.25">
@@ -2426,7 +2425,7 @@
       </c>
       <c r="F19" t="str">
         <f t="shared" si="0"/>
-        <v>18, subsection, 2, Beleuchtung, ,</v>
+        <v>18, subsection, 2, {Beleuchtung}, a,</v>
       </c>
     </row>
     <row r="20" spans="2:6" x14ac:dyDescent="0.25">
@@ -2438,7 +2437,7 @@
       </c>
       <c r="F20" t="str">
         <f t="shared" si="0"/>
-        <v>18, subsection, 2, Wärmequellen, ,</v>
+        <v>18, subsection, 2, {Wärmequellen}, a,</v>
       </c>
     </row>
     <row r="21" spans="2:6" x14ac:dyDescent="0.25">
@@ -2450,7 +2449,7 @@
       </c>
       <c r="F21" t="str">
         <f t="shared" si="0"/>
-        <v>18, subsection, 2, Trinkwarmwasser, ,</v>
+        <v>18, subsection, 2, {Trinkwarmwasser}, a,</v>
       </c>
     </row>
     <row r="22" spans="2:6" x14ac:dyDescent="0.25">
@@ -2462,7 +2461,7 @@
       </c>
       <c r="F22" t="str">
         <f t="shared" si="0"/>
-        <v>18, subsection, 2, Gezielter Luftaustausch mit Zone Pfangutlager, ,</v>
+        <v>18, subsection, 2, {Gezielter Luftaustausch mit Zone Pfangutlager}, a,</v>
       </c>
     </row>
     <row r="23" spans="2:6" x14ac:dyDescent="0.25">
@@ -2474,7 +2473,7 @@
       </c>
       <c r="F23" t="str">
         <f t="shared" si="0"/>
-        <v>19, subsection, 2, Konfiguration Lüftungsanlage, ,</v>
+        <v>19, subsection, 2, {Konfiguration Lüftungsanlage}, a,</v>
       </c>
     </row>
     <row r="24" spans="2:6" x14ac:dyDescent="0.25">
@@ -2486,7 +2485,7 @@
       </c>
       <c r="F24" t="str">
         <f t="shared" si="0"/>
-        <v>26, subsection, 2, Berechnung / Ergebnisse, ,</v>
+        <v>26, subsection, 2, {Berechnung / Ergebnisse}, a,</v>
       </c>
     </row>
     <row r="25" spans="2:6" x14ac:dyDescent="0.25">
@@ -2498,7 +2497,7 @@
       </c>
       <c r="F25" t="str">
         <f t="shared" si="0"/>
-        <v>29, section, 1, Zone Lager, ,</v>
+        <v>29, section, 1, {Zone Lager}, a,</v>
       </c>
     </row>
     <row r="26" spans="2:6" x14ac:dyDescent="0.25">
@@ -2510,7 +2509,7 @@
       </c>
       <c r="F26" t="str">
         <f t="shared" si="0"/>
-        <v>29, subsection, 2, Geometrie, ,</v>
+        <v>29, subsection, 2, {Geometrie}, a,</v>
       </c>
     </row>
     <row r="27" spans="2:6" x14ac:dyDescent="0.25">
@@ -2522,7 +2521,7 @@
       </c>
       <c r="F27" t="str">
         <f t="shared" si="0"/>
-        <v>30, subsection, 2, Raumliste, ,</v>
+        <v>30, subsection, 2, {Raumliste}, a,</v>
       </c>
     </row>
     <row r="28" spans="2:6" x14ac:dyDescent="0.25">
@@ -2534,7 +2533,7 @@
       </c>
       <c r="F28" t="str">
         <f t="shared" si="0"/>
-        <v>30, subsection, 2, Randbedingungen, ,</v>
+        <v>30, subsection, 2, {Randbedingungen}, a,</v>
       </c>
     </row>
     <row r="29" spans="2:6" x14ac:dyDescent="0.25">
@@ -2546,7 +2545,7 @@
       </c>
       <c r="F29" t="str">
         <f t="shared" si="0"/>
-        <v>30, subsection, 2, Luftwechsel, ,</v>
+        <v>30, subsection, 2, {Luftwechsel}, a,</v>
       </c>
     </row>
     <row r="30" spans="2:6" x14ac:dyDescent="0.25">
@@ -2558,7 +2557,7 @@
       </c>
       <c r="F30" t="str">
         <f t="shared" si="0"/>
-        <v>30, subsection, 2, Nutzungszeiten, ,</v>
+        <v>30, subsection, 2, {Nutzungszeiten}, a,</v>
       </c>
     </row>
     <row r="31" spans="2:6" x14ac:dyDescent="0.25">
@@ -2570,7 +2569,7 @@
       </c>
       <c r="F31" t="str">
         <f t="shared" si="0"/>
-        <v>30, subsection, 2, Heizung, ,</v>
+        <v>30, subsection, 2, {Heizung}, a,</v>
       </c>
     </row>
     <row r="32" spans="2:6" x14ac:dyDescent="0.25">
@@ -2582,7 +2581,7 @@
       </c>
       <c r="F32" t="str">
         <f t="shared" si="0"/>
-        <v>31, subsection, 2, Beleuchtung, ,</v>
+        <v>31, subsection, 2, {Beleuchtung}, a,</v>
       </c>
     </row>
     <row r="33" spans="2:6" x14ac:dyDescent="0.25">
@@ -2594,7 +2593,7 @@
       </c>
       <c r="F33" t="str">
         <f t="shared" si="0"/>
-        <v>31, subsection, 2, Wärmequellen, ,</v>
+        <v>31, subsection, 2, {Wärmequellen}, a,</v>
       </c>
     </row>
     <row r="34" spans="2:6" x14ac:dyDescent="0.25">
@@ -2606,7 +2605,7 @@
       </c>
       <c r="F34" t="str">
         <f t="shared" si="0"/>
-        <v>35, subsection, 2, Berechnung / Ergebnisse, ,</v>
+        <v>35, subsection, 2, {Berechnung / Ergebnisse}, a,</v>
       </c>
     </row>
     <row r="35" spans="2:6" x14ac:dyDescent="0.25">
@@ -2618,7 +2617,7 @@
       </c>
       <c r="F35" t="str">
         <f t="shared" si="0"/>
-        <v>38, section, 1, Zone Technik, ,</v>
+        <v>38, section, 1, {Zone Technik}, a,</v>
       </c>
     </row>
     <row r="36" spans="2:6" x14ac:dyDescent="0.25">
@@ -2630,7 +2629,7 @@
       </c>
       <c r="F36" t="str">
         <f t="shared" si="0"/>
-        <v>38, subsection, 2, Geometrie, ,</v>
+        <v>38, subsection, 2, {Geometrie}, a,</v>
       </c>
     </row>
     <row r="37" spans="2:6" x14ac:dyDescent="0.25">
@@ -2642,7 +2641,7 @@
       </c>
       <c r="F37" t="str">
         <f t="shared" si="0"/>
-        <v>39, subsection, 2, Raumliste, ,</v>
+        <v>39, subsection, 2, {Raumliste}, a,</v>
       </c>
     </row>
     <row r="38" spans="2:6" x14ac:dyDescent="0.25">
@@ -2654,7 +2653,7 @@
       </c>
       <c r="F38" t="str">
         <f t="shared" si="0"/>
-        <v>39, subsection, 2, Randbedingungen, ,</v>
+        <v>39, subsection, 2, {Randbedingungen}, a,</v>
       </c>
     </row>
     <row r="39" spans="2:6" x14ac:dyDescent="0.25">
@@ -2666,7 +2665,7 @@
       </c>
       <c r="F39" t="str">
         <f t="shared" si="0"/>
-        <v>39, subsection, 2, Luftwechsel, ,</v>
+        <v>39, subsection, 2, {Luftwechsel}, a,</v>
       </c>
     </row>
     <row r="40" spans="2:6" x14ac:dyDescent="0.25">
@@ -2678,7 +2677,7 @@
       </c>
       <c r="F40" t="str">
         <f t="shared" si="0"/>
-        <v>39, subsection, 2, Nutzungszeiten, ,</v>
+        <v>39, subsection, 2, {Nutzungszeiten}, a,</v>
       </c>
     </row>
     <row r="41" spans="2:6" x14ac:dyDescent="0.25">
@@ -2690,7 +2689,7 @@
       </c>
       <c r="F41" t="str">
         <f t="shared" si="0"/>
-        <v>39, subsection, 2, Heizung, ,</v>
+        <v>39, subsection, 2, {Heizung}, a,</v>
       </c>
     </row>
     <row r="42" spans="2:6" x14ac:dyDescent="0.25">
@@ -2702,7 +2701,7 @@
       </c>
       <c r="F42" t="str">
         <f t="shared" si="0"/>
-        <v>40, subsection, 2, Beleuchtung, ,</v>
+        <v>40, subsection, 2, {Beleuchtung}, a,</v>
       </c>
     </row>
     <row r="43" spans="2:6" x14ac:dyDescent="0.25">
@@ -2714,7 +2713,7 @@
       </c>
       <c r="F43" t="str">
         <f t="shared" si="0"/>
-        <v>40, subsection, 2, Wärmequellen, ,</v>
+        <v>40, subsection, 2, {Wärmequellen}, a,</v>
       </c>
     </row>
     <row r="44" spans="2:6" x14ac:dyDescent="0.25">
@@ -2726,7 +2725,7 @@
       </c>
       <c r="F44" t="str">
         <f t="shared" si="0"/>
-        <v>44, subsection, 2, Berechnung / Ergebnisse, ,</v>
+        <v>44, subsection, 2, {Berechnung / Ergebnisse}, a,</v>
       </c>
     </row>
     <row r="45" spans="2:6" x14ac:dyDescent="0.25">
@@ -2738,7 +2737,7 @@
       </c>
       <c r="F45" t="str">
         <f t="shared" si="0"/>
-        <v>47, section, 1, Zone Aufenthaltsraum, ,</v>
+        <v>47, section, 1, {Zone Aufenthaltsraum}, a,</v>
       </c>
     </row>
     <row r="46" spans="2:6" x14ac:dyDescent="0.25">
@@ -2750,7 +2749,7 @@
       </c>
       <c r="F46" t="str">
         <f t="shared" si="0"/>
-        <v>47, subsection, 2, Geometrie, ,</v>
+        <v>47, subsection, 2, {Geometrie}, a,</v>
       </c>
     </row>
     <row r="47" spans="2:6" x14ac:dyDescent="0.25">
@@ -2762,7 +2761,7 @@
       </c>
       <c r="F47" t="str">
         <f t="shared" si="0"/>
-        <v>48, subsection, 2, Raumliste, ,</v>
+        <v>48, subsection, 2, {Raumliste}, a,</v>
       </c>
     </row>
     <row r="48" spans="2:6" x14ac:dyDescent="0.25">
@@ -2774,7 +2773,7 @@
       </c>
       <c r="F48" t="str">
         <f t="shared" si="0"/>
-        <v>48, subsection, 2, Randbedingungen, ,</v>
+        <v>48, subsection, 2, {Randbedingungen}, a,</v>
       </c>
     </row>
     <row r="49" spans="2:6" x14ac:dyDescent="0.25">
@@ -2786,7 +2785,7 @@
       </c>
       <c r="F49" t="str">
         <f t="shared" si="0"/>
-        <v>48, subsection, 2, Luftwechsel, ,</v>
+        <v>48, subsection, 2, {Luftwechsel}, a,</v>
       </c>
     </row>
     <row r="50" spans="2:6" x14ac:dyDescent="0.25">
@@ -2798,7 +2797,7 @@
       </c>
       <c r="F50" t="str">
         <f t="shared" si="0"/>
-        <v>48, subsection, 2, Nutzungszeiten, ,</v>
+        <v>48, subsection, 2, {Nutzungszeiten}, a,</v>
       </c>
     </row>
     <row r="51" spans="2:6" x14ac:dyDescent="0.25">
@@ -2810,7 +2809,7 @@
       </c>
       <c r="F51" t="str">
         <f t="shared" si="0"/>
-        <v>48, subsection, 2, Heizung, ,</v>
+        <v>48, subsection, 2, {Heizung}, a,</v>
       </c>
     </row>
     <row r="52" spans="2:6" x14ac:dyDescent="0.25">
@@ -2822,7 +2821,7 @@
       </c>
       <c r="F52" t="str">
         <f t="shared" si="0"/>
-        <v>49, subsection, 2, Kühlung, ,</v>
+        <v>49, subsection, 2, {Kühlung}, a,</v>
       </c>
     </row>
     <row r="53" spans="2:6" x14ac:dyDescent="0.25">
@@ -2834,7 +2833,7 @@
       </c>
       <c r="F53" t="str">
         <f t="shared" si="0"/>
-        <v>49, subsection, 2, Beleuchtung, ,</v>
+        <v>49, subsection, 2, {Beleuchtung}, a,</v>
       </c>
     </row>
     <row r="54" spans="2:6" x14ac:dyDescent="0.25">
@@ -2846,7 +2845,7 @@
       </c>
       <c r="F54" t="str">
         <f t="shared" si="0"/>
-        <v>49, subsection, 2, Wärmequellen, ,</v>
+        <v>49, subsection, 2, {Wärmequellen}, a,</v>
       </c>
     </row>
     <row r="55" spans="2:6" x14ac:dyDescent="0.25">
@@ -2858,7 +2857,7 @@
       </c>
       <c r="F55" t="str">
         <f t="shared" si="0"/>
-        <v>56, subsection, 2, Berechnung / Ergebnisse, ,</v>
+        <v>56, subsection, 2, {Berechnung / Ergebnisse}, a,</v>
       </c>
     </row>
     <row r="56" spans="2:6" x14ac:dyDescent="0.25">
@@ -2870,7 +2869,7 @@
       </c>
       <c r="F56" t="str">
         <f t="shared" si="0"/>
-        <v>59, section, 1, Zone Pfandgutlager, ,</v>
+        <v>59, section, 1, {Zone Pfandgutlager}, a,</v>
       </c>
     </row>
     <row r="57" spans="2:6" x14ac:dyDescent="0.25">
@@ -2882,7 +2881,7 @@
       </c>
       <c r="F57" t="str">
         <f t="shared" si="0"/>
-        <v>59, subsection, 2, Geometrie, ,</v>
+        <v>59, subsection, 2, {Geometrie}, a,</v>
       </c>
     </row>
     <row r="58" spans="2:6" x14ac:dyDescent="0.25">
@@ -2894,7 +2893,7 @@
       </c>
       <c r="F58" t="str">
         <f t="shared" si="0"/>
-        <v>60, subsection, 2, Raumliste, ,</v>
+        <v>60, subsection, 2, {Raumliste}, a,</v>
       </c>
     </row>
     <row r="59" spans="2:6" x14ac:dyDescent="0.25">
@@ -2906,7 +2905,7 @@
       </c>
       <c r="F59" t="str">
         <f t="shared" si="0"/>
-        <v>60, subsection, 2, Randbedingungen, ,</v>
+        <v>60, subsection, 2, {Randbedingungen}, a,</v>
       </c>
     </row>
     <row r="60" spans="2:6" x14ac:dyDescent="0.25">
@@ -2918,7 +2917,7 @@
       </c>
       <c r="F60" t="str">
         <f t="shared" si="0"/>
-        <v>60, subsection, 2, Luftwechsel, ,</v>
+        <v>60, subsection, 2, {Luftwechsel}, a,</v>
       </c>
     </row>
     <row r="61" spans="2:6" x14ac:dyDescent="0.25">
@@ -2930,7 +2929,7 @@
       </c>
       <c r="F61" t="str">
         <f t="shared" si="0"/>
-        <v>60, subsection, 2, Nutzungszeiten, ,</v>
+        <v>60, subsection, 2, {Nutzungszeiten}, a,</v>
       </c>
     </row>
     <row r="62" spans="2:6" x14ac:dyDescent="0.25">
@@ -2942,7 +2941,7 @@
       </c>
       <c r="F62" t="str">
         <f t="shared" si="0"/>
-        <v>60, subsection, 2, Heizung, ,</v>
+        <v>60, subsection, 2, {Heizung}, a,</v>
       </c>
     </row>
     <row r="63" spans="2:6" x14ac:dyDescent="0.25">
@@ -2954,7 +2953,7 @@
       </c>
       <c r="F63" t="str">
         <f t="shared" si="0"/>
-        <v>61, subsection, 2, Lüftung, ,</v>
+        <v>61, subsection, 2, {Lüftung}, a,</v>
       </c>
     </row>
     <row r="64" spans="2:6" x14ac:dyDescent="0.25">
@@ -2966,7 +2965,7 @@
       </c>
       <c r="F64" t="str">
         <f t="shared" si="0"/>
-        <v>61, subsection, 2, Beleuchtung, ,</v>
+        <v>61, subsection, 2, {Beleuchtung}, a,</v>
       </c>
     </row>
     <row r="65" spans="2:6" x14ac:dyDescent="0.25">
@@ -2978,7 +2977,7 @@
       </c>
       <c r="F65" t="str">
         <f t="shared" si="0"/>
-        <v>61, subsection, 2, Wärmequellen, ,</v>
+        <v>61, subsection, 2, {Wärmequellen}, a,</v>
       </c>
     </row>
     <row r="66" spans="2:6" x14ac:dyDescent="0.25">
@@ -2990,7 +2989,7 @@
       </c>
       <c r="F66" t="str">
         <f t="shared" si="0"/>
-        <v>61, subsection, 2, Gezielter Luftaustausch mit Zone Pfangutlager, ,</v>
+        <v>61, subsection, 2, {Gezielter Luftaustausch mit Zone Pfangutlager}, a,</v>
       </c>
     </row>
     <row r="67" spans="2:6" x14ac:dyDescent="0.25">
@@ -3002,7 +3001,7 @@
       </c>
       <c r="F67" t="str">
         <f t="shared" si="0"/>
-        <v>61, subsection, 2, Konfiguration Lüftungsanlage, ,</v>
+        <v>61, subsection, 2, {Konfiguration Lüftungsanlage}, a,</v>
       </c>
     </row>
     <row r="68" spans="2:6" x14ac:dyDescent="0.25">
@@ -3014,7 +3013,7 @@
       </c>
       <c r="F68" t="str">
         <f t="shared" si="0"/>
-        <v>65, subsection, 2, Berechnung / Ergebnisse, ,</v>
+        <v>65, subsection, 2, {Berechnung / Ergebnisse}, a,</v>
       </c>
     </row>
     <row r="69" spans="2:6" x14ac:dyDescent="0.25">
@@ -3025,8 +3024,8 @@
         <v>68</v>
       </c>
       <c r="F69" t="str">
-        <f t="shared" ref="F69:F129" si="1">CONCATENATE(D69,", ",IF(ISBLANK(A69)=FALSE,A$3,IF(ISBLANK(B69)=FALSE,B$3,C$3)),", ",IF(ISBLANK(A69)=FALSE,0,IF(ISBLANK(B69)=FALSE,1,2)),", ",IF(ISBLANK(A69)=FALSE,A69,IF(ISBLANK(B69)=FALSE,B69,C69)),IF(ISBLANK(D70)=TRUE,",",", ,"))</f>
-        <v>68, section, 1, Zone Aktenraum, ,</v>
+        <f t="shared" ref="F69:F129" si="1">CONCATENATE(D69,", ",IF(ISBLANK(A69)=FALSE,A$3,IF(ISBLANK(B69)=FALSE,B$3,C$3)),", ",IF(ISBLANK(A69)=FALSE,0,IF(ISBLANK(B69)=FALSE,1,2)),", {",IF(ISBLANK(A69)=FALSE,A69,IF(ISBLANK(B69)=FALSE,B69,C69)),"}, a",IF(ISBLANK(D70)=TRUE,"",","))</f>
+        <v>68, section, 1, {Zone Aktenraum}, a,</v>
       </c>
     </row>
     <row r="70" spans="2:6" x14ac:dyDescent="0.25">
@@ -3038,7 +3037,7 @@
       </c>
       <c r="F70" t="str">
         <f t="shared" si="1"/>
-        <v>68, subsection, 2, Geometrie, ,</v>
+        <v>68, subsection, 2, {Geometrie}, a,</v>
       </c>
     </row>
     <row r="71" spans="2:6" x14ac:dyDescent="0.25">
@@ -3050,7 +3049,7 @@
       </c>
       <c r="F71" t="str">
         <f t="shared" si="1"/>
-        <v>69, subsection, 2, Raumliste, ,</v>
+        <v>69, subsection, 2, {Raumliste}, a,</v>
       </c>
     </row>
     <row r="72" spans="2:6" x14ac:dyDescent="0.25">
@@ -3062,7 +3061,7 @@
       </c>
       <c r="F72" t="str">
         <f t="shared" si="1"/>
-        <v>69, subsection, 2, Randbedingungen, ,</v>
+        <v>69, subsection, 2, {Randbedingungen}, a,</v>
       </c>
     </row>
     <row r="73" spans="2:6" x14ac:dyDescent="0.25">
@@ -3074,7 +3073,7 @@
       </c>
       <c r="F73" t="str">
         <f t="shared" si="1"/>
-        <v>69, subsection, 2, Luftwechsel, ,</v>
+        <v>69, subsection, 2, {Luftwechsel}, a,</v>
       </c>
     </row>
     <row r="74" spans="2:6" x14ac:dyDescent="0.25">
@@ -3086,7 +3085,7 @@
       </c>
       <c r="F74" t="str">
         <f t="shared" si="1"/>
-        <v>69, subsection, 2, Nutzungszeiten, ,</v>
+        <v>69, subsection, 2, {Nutzungszeiten}, a,</v>
       </c>
     </row>
     <row r="75" spans="2:6" x14ac:dyDescent="0.25">
@@ -3098,7 +3097,7 @@
       </c>
       <c r="F75" t="str">
         <f t="shared" si="1"/>
-        <v>69, subsection, 2, Heizung, ,</v>
+        <v>69, subsection, 2, {Heizung}, a,</v>
       </c>
     </row>
     <row r="76" spans="2:6" x14ac:dyDescent="0.25">
@@ -3110,7 +3109,7 @@
       </c>
       <c r="F76" t="str">
         <f t="shared" si="1"/>
-        <v>70, subsection, 2, Kühlung, ,</v>
+        <v>70, subsection, 2, {Kühlung}, a,</v>
       </c>
     </row>
     <row r="77" spans="2:6" x14ac:dyDescent="0.25">
@@ -3122,7 +3121,7 @@
       </c>
       <c r="F77" t="str">
         <f t="shared" si="1"/>
-        <v>70, subsection, 2, Lüftung, ,</v>
+        <v>70, subsection, 2, {Lüftung}, a,</v>
       </c>
     </row>
     <row r="78" spans="2:6" x14ac:dyDescent="0.25">
@@ -3134,7 +3133,7 @@
       </c>
       <c r="F78" t="str">
         <f t="shared" si="1"/>
-        <v>70, subsection, 2, Beleuchtung, ,</v>
+        <v>70, subsection, 2, {Beleuchtung}, a,</v>
       </c>
     </row>
     <row r="79" spans="2:6" x14ac:dyDescent="0.25">
@@ -3146,7 +3145,7 @@
       </c>
       <c r="F79" t="str">
         <f t="shared" si="1"/>
-        <v>70, subsection, 2, Wärmequellen, ,</v>
+        <v>70, subsection, 2, {Wärmequellen}, a,</v>
       </c>
     </row>
     <row r="80" spans="2:6" x14ac:dyDescent="0.25">
@@ -3158,7 +3157,7 @@
       </c>
       <c r="F80" t="str">
         <f t="shared" si="1"/>
-        <v>70, subsection, 2, Konfiguration Lüftungsanlage, ,</v>
+        <v>70, subsection, 2, {Konfiguration Lüftungsanlage}, a,</v>
       </c>
     </row>
     <row r="81" spans="2:6" x14ac:dyDescent="0.25">
@@ -3170,7 +3169,7 @@
       </c>
       <c r="F81" t="str">
         <f t="shared" si="1"/>
-        <v>78, subsection, 2, Berechnung / Ergebnisse, ,</v>
+        <v>78, subsection, 2, {Berechnung / Ergebnisse}, a,</v>
       </c>
     </row>
     <row r="82" spans="2:6" x14ac:dyDescent="0.25">
@@ -3182,7 +3181,7 @@
       </c>
       <c r="F82" t="str">
         <f t="shared" si="1"/>
-        <v>81, section, 1, Zone WC, Umkleide, ,</v>
+        <v>81, section, 1, {Zone WC, Umkleide}, a,</v>
       </c>
     </row>
     <row r="83" spans="2:6" x14ac:dyDescent="0.25">
@@ -3194,7 +3193,7 @@
       </c>
       <c r="F83" t="str">
         <f t="shared" si="1"/>
-        <v>81, subsection, 2, Geometrie, ,</v>
+        <v>81, subsection, 2, {Geometrie}, a,</v>
       </c>
     </row>
     <row r="84" spans="2:6" x14ac:dyDescent="0.25">
@@ -3206,7 +3205,7 @@
       </c>
       <c r="F84" t="str">
         <f t="shared" si="1"/>
-        <v>82, subsection, 2, Raumliste, ,</v>
+        <v>82, subsection, 2, {Raumliste}, a,</v>
       </c>
     </row>
     <row r="85" spans="2:6" x14ac:dyDescent="0.25">
@@ -3218,7 +3217,7 @@
       </c>
       <c r="F85" t="str">
         <f t="shared" si="1"/>
-        <v>82, subsection, 2, Randbedingungen, ,</v>
+        <v>82, subsection, 2, {Randbedingungen}, a,</v>
       </c>
     </row>
     <row r="86" spans="2:6" x14ac:dyDescent="0.25">
@@ -3230,7 +3229,7 @@
       </c>
       <c r="F86" t="str">
         <f t="shared" si="1"/>
-        <v>82, subsection, 2, Luftwechsel, ,</v>
+        <v>82, subsection, 2, {Luftwechsel}, a,</v>
       </c>
     </row>
     <row r="87" spans="2:6" x14ac:dyDescent="0.25">
@@ -3242,7 +3241,7 @@
       </c>
       <c r="F87" t="str">
         <f t="shared" si="1"/>
-        <v>82, subsection, 2, Nutzungszeiten, ,</v>
+        <v>82, subsection, 2, {Nutzungszeiten}, a,</v>
       </c>
     </row>
     <row r="88" spans="2:6" x14ac:dyDescent="0.25">
@@ -3254,7 +3253,7 @@
       </c>
       <c r="F88" t="str">
         <f t="shared" si="1"/>
-        <v>83, subsection, 2, Heizung, ,</v>
+        <v>83, subsection, 2, {Heizung}, a,</v>
       </c>
     </row>
     <row r="89" spans="2:6" x14ac:dyDescent="0.25">
@@ -3266,7 +3265,7 @@
       </c>
       <c r="F89" t="str">
         <f t="shared" si="1"/>
-        <v>83, subsection, 2, Lüftung, ,</v>
+        <v>83, subsection, 2, {Lüftung}, a,</v>
       </c>
     </row>
     <row r="90" spans="2:6" x14ac:dyDescent="0.25">
@@ -3278,7 +3277,7 @@
       </c>
       <c r="F90" t="str">
         <f t="shared" si="1"/>
-        <v>83, subsection, 2, Beleuchtung, ,</v>
+        <v>83, subsection, 2, {Beleuchtung}, a,</v>
       </c>
     </row>
     <row r="91" spans="2:6" x14ac:dyDescent="0.25">
@@ -3290,7 +3289,7 @@
       </c>
       <c r="F91" t="str">
         <f t="shared" si="1"/>
-        <v>83, subsection, 2, Wärmequellen, ,</v>
+        <v>83, subsection, 2, {Wärmequellen}, a,</v>
       </c>
     </row>
     <row r="92" spans="2:6" x14ac:dyDescent="0.25">
@@ -3302,7 +3301,7 @@
       </c>
       <c r="F92" t="str">
         <f t="shared" si="1"/>
-        <v>83, subsection, 2, Konfiguration Lüftungsanlage, ,</v>
+        <v>83, subsection, 2, {Konfiguration Lüftungsanlage}, a,</v>
       </c>
     </row>
     <row r="93" spans="2:6" x14ac:dyDescent="0.25">
@@ -3314,7 +3313,7 @@
       </c>
       <c r="F93" t="str">
         <f t="shared" si="1"/>
-        <v>88, subsection, 2, Berechnung / Ergebnisse, ,</v>
+        <v>88, subsection, 2, {Berechnung / Ergebnisse}, a,</v>
       </c>
     </row>
     <row r="94" spans="2:6" x14ac:dyDescent="0.25">
@@ -3326,7 +3325,7 @@
       </c>
       <c r="F94" t="str">
         <f t="shared" si="1"/>
-        <v>91, section, 1, Zone RVL Büro, ,</v>
+        <v>91, section, 1, {Zone RVL Büro}, a,</v>
       </c>
     </row>
     <row r="95" spans="2:6" x14ac:dyDescent="0.25">
@@ -3338,7 +3337,7 @@
       </c>
       <c r="F95" t="str">
         <f t="shared" si="1"/>
-        <v>91, subsection, 2, Geometrie, ,</v>
+        <v>91, subsection, 2, {Geometrie}, a,</v>
       </c>
     </row>
     <row r="96" spans="2:6" x14ac:dyDescent="0.25">
@@ -3350,7 +3349,7 @@
       </c>
       <c r="F96" t="str">
         <f t="shared" si="1"/>
-        <v>92, subsection, 2, Raumliste, ,</v>
+        <v>92, subsection, 2, {Raumliste}, a,</v>
       </c>
     </row>
     <row r="97" spans="2:6" x14ac:dyDescent="0.25">
@@ -3362,7 +3361,7 @@
       </c>
       <c r="F97" t="str">
         <f t="shared" si="1"/>
-        <v>92, subsection, 2, Randbedingungen, ,</v>
+        <v>92, subsection, 2, {Randbedingungen}, a,</v>
       </c>
     </row>
     <row r="98" spans="2:6" x14ac:dyDescent="0.25">
@@ -3374,7 +3373,7 @@
       </c>
       <c r="F98" t="str">
         <f t="shared" si="1"/>
-        <v>92, subsection, 2, Luftwechsel, ,</v>
+        <v>92, subsection, 2, {Luftwechsel}, a,</v>
       </c>
     </row>
     <row r="99" spans="2:6" x14ac:dyDescent="0.25">
@@ -3386,7 +3385,7 @@
       </c>
       <c r="F99" t="str">
         <f t="shared" si="1"/>
-        <v>92, subsection, 2, Nutzungszeiten, ,</v>
+        <v>92, subsection, 2, {Nutzungszeiten}, a,</v>
       </c>
     </row>
     <row r="100" spans="2:6" x14ac:dyDescent="0.25">
@@ -3398,7 +3397,7 @@
       </c>
       <c r="F100" t="str">
         <f t="shared" si="1"/>
-        <v>92, subsection, 2, Heizung, ,</v>
+        <v>92, subsection, 2, {Heizung}, a,</v>
       </c>
     </row>
     <row r="101" spans="2:6" x14ac:dyDescent="0.25">
@@ -3410,7 +3409,7 @@
       </c>
       <c r="F101" t="str">
         <f t="shared" si="1"/>
-        <v>93, subsection, 2, Kühlung, ,</v>
+        <v>93, subsection, 2, {Kühlung}, a,</v>
       </c>
     </row>
     <row r="102" spans="2:6" x14ac:dyDescent="0.25">
@@ -3422,7 +3421,7 @@
       </c>
       <c r="F102" t="str">
         <f t="shared" si="1"/>
-        <v>93, subsection, 2, Beleuchtung, ,</v>
+        <v>93, subsection, 2, {Beleuchtung}, a,</v>
       </c>
     </row>
     <row r="103" spans="2:6" x14ac:dyDescent="0.25">
@@ -3434,7 +3433,7 @@
       </c>
       <c r="F103" t="str">
         <f t="shared" si="1"/>
-        <v>93, subsection, 2, Wärmequellen, ,</v>
+        <v>93, subsection, 2, {Wärmequellen}, a,</v>
       </c>
     </row>
     <row r="104" spans="2:6" x14ac:dyDescent="0.25">
@@ -3446,7 +3445,7 @@
       </c>
       <c r="F104" t="str">
         <f t="shared" si="1"/>
-        <v>100, subsection, 2, Berechnung / Ergebnisse, ,</v>
+        <v>100, subsection, 2, {Berechnung / Ergebnisse}, a,</v>
       </c>
     </row>
     <row r="105" spans="2:6" x14ac:dyDescent="0.25">
@@ -3458,7 +3457,7 @@
       </c>
       <c r="F105" t="str">
         <f t="shared" si="1"/>
-        <v>103, section, 1, Zone Dachraum, ,</v>
+        <v>103, section, 1, {Zone Dachraum}, a,</v>
       </c>
     </row>
     <row r="106" spans="2:6" x14ac:dyDescent="0.25">
@@ -3470,7 +3469,7 @@
       </c>
       <c r="F106" t="str">
         <f t="shared" si="1"/>
-        <v>103, subsection, 2, Geometrie, ,</v>
+        <v>103, subsection, 2, {Geometrie}, a,</v>
       </c>
     </row>
     <row r="107" spans="2:6" x14ac:dyDescent="0.25">
@@ -3482,7 +3481,7 @@
       </c>
       <c r="F107" t="str">
         <f t="shared" si="1"/>
-        <v>104, subsection, 2, Raumliste, ,</v>
+        <v>104, subsection, 2, {Raumliste}, a,</v>
       </c>
     </row>
     <row r="108" spans="2:6" x14ac:dyDescent="0.25">
@@ -3494,7 +3493,7 @@
       </c>
       <c r="F108" t="str">
         <f t="shared" si="1"/>
-        <v>104, subsection, 2, Randbedingungen, ,</v>
+        <v>104, subsection, 2, {Randbedingungen}, a,</v>
       </c>
     </row>
     <row r="109" spans="2:6" x14ac:dyDescent="0.25">
@@ -3506,7 +3505,7 @@
       </c>
       <c r="F109" t="str">
         <f t="shared" si="1"/>
-        <v>104, subsection, 2, Luftwechsel, ,</v>
+        <v>104, subsection, 2, {Luftwechsel}, a,</v>
       </c>
     </row>
     <row r="110" spans="2:6" x14ac:dyDescent="0.25">
@@ -3518,7 +3517,7 @@
       </c>
       <c r="F110" t="str">
         <f t="shared" si="1"/>
-        <v>104, subsection, 2, Nutzungszeiten, ,</v>
+        <v>104, subsection, 2, {Nutzungszeiten}, a,</v>
       </c>
     </row>
     <row r="111" spans="2:6" x14ac:dyDescent="0.25">
@@ -3530,7 +3529,7 @@
       </c>
       <c r="F111" t="str">
         <f t="shared" si="1"/>
-        <v>104, subsection, 2, Beleuchtung, ,</v>
+        <v>104, subsection, 2, {Beleuchtung}, a,</v>
       </c>
     </row>
     <row r="112" spans="2:6" x14ac:dyDescent="0.25">
@@ -3542,7 +3541,7 @@
       </c>
       <c r="F112" t="str">
         <f t="shared" si="1"/>
-        <v>105, subsection, 2, Wärmequellen, ,</v>
+        <v>105, subsection, 2, {Wärmequellen}, a,</v>
       </c>
     </row>
     <row r="113" spans="2:6" x14ac:dyDescent="0.25">
@@ -3554,7 +3553,7 @@
       </c>
       <c r="F113" t="str">
         <f t="shared" si="1"/>
-        <v>106, subsection, 2, Berechnung / Ergebnisse, ,</v>
+        <v>106, subsection, 2, {Berechnung / Ergebnisse}, a,</v>
       </c>
     </row>
     <row r="114" spans="2:6" x14ac:dyDescent="0.25">
@@ -3566,7 +3565,7 @@
       </c>
       <c r="F114" t="str">
         <f t="shared" si="1"/>
-        <v>108, section, 1, Anlagentechnik, ,</v>
+        <v>108, section, 1, {Anlagentechnik}, a,</v>
       </c>
     </row>
     <row r="115" spans="2:6" x14ac:dyDescent="0.25">
@@ -3578,7 +3577,7 @@
       </c>
       <c r="F115" t="str">
         <f t="shared" si="1"/>
-        <v>108, subsection, 2, Heizungsanlage, ,</v>
+        <v>108, subsection, 2, {Heizungsanlage}, a,</v>
       </c>
     </row>
     <row r="116" spans="2:6" x14ac:dyDescent="0.25">
@@ -3590,7 +3589,7 @@
       </c>
       <c r="F116" t="str">
         <f t="shared" si="1"/>
-        <v>111, subsection, 2, Trinkwasseranlage, ,</v>
+        <v>111, subsection, 2, {Trinkwasseranlage}, a,</v>
       </c>
     </row>
     <row r="117" spans="2:6" x14ac:dyDescent="0.25">
@@ -3602,7 +3601,7 @@
       </c>
       <c r="F117" t="str">
         <f t="shared" si="1"/>
-        <v>112, subsection, 2, Kühlungsanlage, ,</v>
+        <v>112, subsection, 2, {Kühlungsanlage}, a,</v>
       </c>
     </row>
     <row r="118" spans="2:6" x14ac:dyDescent="0.25">
@@ -3614,7 +3613,7 @@
       </c>
       <c r="F118" t="str">
         <f t="shared" si="1"/>
-        <v>114, subsection, 2, RLT-Anlage, ,</v>
+        <v>114, subsection, 2, {RLT-Anlage}, a,</v>
       </c>
     </row>
     <row r="119" spans="2:6" x14ac:dyDescent="0.25">
@@ -3626,7 +3625,7 @@
       </c>
       <c r="F119" t="str">
         <f t="shared" si="1"/>
-        <v>118, section, 1, Beleuchtung, ,</v>
+        <v>118, section, 1, {Beleuchtung}, a,</v>
       </c>
     </row>
     <row r="120" spans="2:6" x14ac:dyDescent="0.25">
@@ -3638,7 +3637,7 @@
       </c>
       <c r="F120" t="str">
         <f t="shared" si="1"/>
-        <v>118, subsection, 2, Verkaufsraum, ,</v>
+        <v>118, subsection, 2, {Verkaufsraum}, a,</v>
       </c>
     </row>
     <row r="121" spans="2:6" x14ac:dyDescent="0.25">
@@ -3650,7 +3649,7 @@
       </c>
       <c r="F121" t="str">
         <f t="shared" si="1"/>
-        <v>118, subsection, 2, Lager, ,</v>
+        <v>118, subsection, 2, {Lager}, a,</v>
       </c>
     </row>
     <row r="122" spans="2:6" x14ac:dyDescent="0.25">
@@ -3662,7 +3661,7 @@
       </c>
       <c r="F122" t="str">
         <f t="shared" si="1"/>
-        <v>118, subsection, 2, Technik, ,</v>
+        <v>118, subsection, 2, {Technik}, a,</v>
       </c>
     </row>
     <row r="123" spans="2:6" x14ac:dyDescent="0.25">
@@ -3674,7 +3673,7 @@
       </c>
       <c r="F123" t="str">
         <f t="shared" si="1"/>
-        <v>119, subsection, 2, Aufenthaltsraum, ,</v>
+        <v>119, subsection, 2, {Aufenthaltsraum}, a,</v>
       </c>
     </row>
     <row r="124" spans="2:6" x14ac:dyDescent="0.25">
@@ -3686,7 +3685,7 @@
       </c>
       <c r="F124" t="str">
         <f t="shared" si="1"/>
-        <v>119, subsection, 2, Pfandgutlager, ,</v>
+        <v>119, subsection, 2, {Pfandgutlager}, a,</v>
       </c>
     </row>
     <row r="125" spans="2:6" x14ac:dyDescent="0.25">
@@ -3698,7 +3697,7 @@
       </c>
       <c r="F125" t="str">
         <f t="shared" si="1"/>
-        <v>120, subsection, 2, Aktenraum, ,</v>
+        <v>120, subsection, 2, {Aktenraum}, a,</v>
       </c>
     </row>
     <row r="126" spans="2:6" x14ac:dyDescent="0.25">
@@ -3710,7 +3709,7 @@
       </c>
       <c r="F126" t="str">
         <f t="shared" si="1"/>
-        <v>120, subsection, 2, WC, Umkleide, ,</v>
+        <v>120, subsection, 2, {WC, Umkleide}, a,</v>
       </c>
     </row>
     <row r="127" spans="2:6" x14ac:dyDescent="0.25">
@@ -3722,7 +3721,7 @@
       </c>
       <c r="F127" t="str">
         <f t="shared" si="1"/>
-        <v>121, subsection, 2, RVL Büro, ,</v>
+        <v>121, subsection, 2, {RVL Büro}, a,</v>
       </c>
     </row>
     <row r="128" spans="2:6" x14ac:dyDescent="0.25">
@@ -3734,7 +3733,7 @@
       </c>
       <c r="F128" t="str">
         <f t="shared" si="1"/>
-        <v>121, subsection, 2, Dachraum, ,</v>
+        <v>121, subsection, 2, {Dachraum}, a,</v>
       </c>
     </row>
     <row r="129" spans="2:6" x14ac:dyDescent="0.25">
@@ -3746,1559 +3745,7 @@
       </c>
       <c r="F129" t="str">
         <f t="shared" si="1"/>
-        <v>123, section, 1, Übersicht der verwendeten Normen und Verordnungen,</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F129"/>
-  <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A94" workbookViewId="0">
-      <selection activeCell="I108" sqref="I108"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="7.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="34.140625" customWidth="1"/>
-    <col min="3" max="3" width="15.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="44.42578125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>0</v>
-      </c>
-      <c r="B3" t="s">
-        <v>1</v>
-      </c>
-      <c r="C3" t="s">
-        <v>2</v>
-      </c>
-      <c r="D3" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B4" t="s">
-        <v>5</v>
-      </c>
-      <c r="D4">
-        <v>2</v>
-      </c>
-      <c r="F4" t="str">
-        <f>CONCATENATE(D4,", ",IF(ISBLANK(A4)=FALSE,A$3,IF(ISBLANK(B4)=FALSE,B$3,C$3)),", ",IF(ISBLANK(A4)=FALSE,0,IF(ISBLANK(B4)=FALSE,1,2)),", ",IF(ISBLANK(A4)=FALSE,A4,IF(ISBLANK(B4)=FALSE,B4,C4)),IF(ISBLANK(D5)=TRUE,",",", ,"))</f>
-        <v>2, section, 1, Allgemeine Angaben zum Gebäude, ,</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="C5" t="s">
-        <v>6</v>
-      </c>
-      <c r="D5">
-        <v>3</v>
-      </c>
-      <c r="F5" t="str">
-        <f t="shared" ref="F5:F68" si="0">CONCATENATE(D5,", ",IF(ISBLANK(A5)=FALSE,A$3,IF(ISBLANK(B5)=FALSE,B$3,C$3)),", ",IF(ISBLANK(A5)=FALSE,0,IF(ISBLANK(B5)=FALSE,1,2)),", ",IF(ISBLANK(A5)=FALSE,A5,IF(ISBLANK(B5)=FALSE,B5,C5)),IF(ISBLANK(D6)=TRUE,",",", ,"))</f>
-        <v>3, subsection, 2, Zonen, ,</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="C6" t="s">
-        <v>8</v>
-      </c>
-      <c r="D6">
-        <v>4</v>
-      </c>
-      <c r="F6" t="str">
-        <f t="shared" si="0"/>
-        <v>4, subsection, 2, Bauteilflächen, ,</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="C7" t="s">
-        <v>9</v>
-      </c>
-      <c r="D7">
-        <v>8</v>
-      </c>
-      <c r="F7" t="str">
-        <f t="shared" si="0"/>
-        <v>8, subsection, 2, Raumliste, ,</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="C8" t="s">
-        <v>10</v>
-      </c>
-      <c r="D8">
-        <v>9</v>
-      </c>
-      <c r="F8" t="str">
-        <f t="shared" si="0"/>
-        <v>9, subsection, 2, Energiebilanz, ,</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B9" t="s">
-        <v>11</v>
-      </c>
-      <c r="D9">
-        <v>15</v>
-      </c>
-      <c r="F9" t="str">
-        <f t="shared" si="0"/>
-        <v>15, section, 1, Bewertung des Gebäudes entsprechend den GEG-Anforderungen, ,</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B10" t="s">
-        <v>12</v>
-      </c>
-      <c r="D10">
-        <v>16</v>
-      </c>
-      <c r="F10" t="str">
-        <f t="shared" si="0"/>
-        <v>16, section, 1, Zone Verkaufsraum, ,</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="C11" t="s">
-        <v>26</v>
-      </c>
-      <c r="D11">
-        <v>16</v>
-      </c>
-      <c r="F11" t="str">
-        <f t="shared" si="0"/>
-        <v>16, subsection, 2, Geometrie, ,</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="C12" t="s">
-        <v>9</v>
-      </c>
-      <c r="D12">
-        <v>17</v>
-      </c>
-      <c r="F12" t="str">
-        <f t="shared" si="0"/>
-        <v>17, subsection, 2, Raumliste, ,</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="C13" t="s">
-        <v>13</v>
-      </c>
-      <c r="D13">
-        <v>17</v>
-      </c>
-      <c r="F13" t="str">
-        <f t="shared" si="0"/>
-        <v>17, subsection, 2, Randbedingungen, ,</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="C14" t="s">
-        <v>14</v>
-      </c>
-      <c r="D14">
-        <v>17</v>
-      </c>
-      <c r="F14" t="str">
-        <f t="shared" si="0"/>
-        <v>17, subsection, 2, Luftwechsel, ,</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="C15" t="s">
-        <v>15</v>
-      </c>
-      <c r="D15">
-        <v>17</v>
-      </c>
-      <c r="F15" t="str">
-        <f t="shared" si="0"/>
-        <v>17, subsection, 2, Nutzungszeiten, ,</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="C16" t="s">
-        <v>16</v>
-      </c>
-      <c r="D16">
-        <v>17</v>
-      </c>
-      <c r="F16" t="str">
-        <f t="shared" si="0"/>
-        <v>17, subsection, 2, Heizung, ,</v>
-      </c>
-    </row>
-    <row r="17" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="C17" t="s">
-        <v>17</v>
-      </c>
-      <c r="D17">
-        <v>18</v>
-      </c>
-      <c r="F17" t="str">
-        <f t="shared" si="0"/>
-        <v>18, subsection, 2, Kühlung, ,</v>
-      </c>
-    </row>
-    <row r="18" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="C18" t="s">
-        <v>18</v>
-      </c>
-      <c r="D18">
-        <v>18</v>
-      </c>
-      <c r="F18" t="str">
-        <f t="shared" si="0"/>
-        <v>18, subsection, 2, Lüftung, ,</v>
-      </c>
-    </row>
-    <row r="19" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="C19" t="s">
-        <v>19</v>
-      </c>
-      <c r="D19">
-        <v>18</v>
-      </c>
-      <c r="F19" t="str">
-        <f t="shared" si="0"/>
-        <v>18, subsection, 2, Beleuchtung, ,</v>
-      </c>
-    </row>
-    <row r="20" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="C20" t="s">
-        <v>20</v>
-      </c>
-      <c r="D20">
-        <v>18</v>
-      </c>
-      <c r="F20" t="str">
-        <f t="shared" si="0"/>
-        <v>18, subsection, 2, Wärmequellen, ,</v>
-      </c>
-    </row>
-    <row r="21" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="C21" t="s">
-        <v>21</v>
-      </c>
-      <c r="D21">
-        <v>18</v>
-      </c>
-      <c r="F21" t="str">
-        <f t="shared" si="0"/>
-        <v>18, subsection, 2, Trinkwarmwasser, ,</v>
-      </c>
-    </row>
-    <row r="22" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="C22" t="s">
-        <v>22</v>
-      </c>
-      <c r="D22">
-        <v>18</v>
-      </c>
-      <c r="F22" t="str">
-        <f t="shared" si="0"/>
-        <v>18, subsection, 2, Gezielter Luftaustausch mit Zone Pfangutlager, ,</v>
-      </c>
-    </row>
-    <row r="23" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="C23" t="s">
-        <v>23</v>
-      </c>
-      <c r="D23">
-        <v>19</v>
-      </c>
-      <c r="F23" t="str">
-        <f t="shared" si="0"/>
-        <v>19, subsection, 2, Konfiguration Lüftungsanlage, ,</v>
-      </c>
-    </row>
-    <row r="24" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="C24" t="s">
-        <v>24</v>
-      </c>
-      <c r="D24">
-        <v>26</v>
-      </c>
-      <c r="F24" t="str">
-        <f t="shared" si="0"/>
-        <v>26, subsection, 2, Berechnung / Ergebnisse, ,</v>
-      </c>
-    </row>
-    <row r="25" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B25" t="s">
-        <v>25</v>
-      </c>
-      <c r="D25">
-        <v>29</v>
-      </c>
-      <c r="F25" t="str">
-        <f t="shared" si="0"/>
-        <v>29, section, 1, Zone Lager, ,</v>
-      </c>
-    </row>
-    <row r="26" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="C26" t="s">
-        <v>26</v>
-      </c>
-      <c r="D26">
-        <v>29</v>
-      </c>
-      <c r="F26" t="str">
-        <f t="shared" si="0"/>
-        <v>29, subsection, 2, Geometrie, ,</v>
-      </c>
-    </row>
-    <row r="27" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="C27" t="s">
-        <v>9</v>
-      </c>
-      <c r="D27">
-        <v>30</v>
-      </c>
-      <c r="F27" t="str">
-        <f t="shared" si="0"/>
-        <v>30, subsection, 2, Raumliste, ,</v>
-      </c>
-    </row>
-    <row r="28" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="C28" t="s">
-        <v>13</v>
-      </c>
-      <c r="D28">
-        <v>30</v>
-      </c>
-      <c r="F28" t="str">
-        <f t="shared" si="0"/>
-        <v>30, subsection, 2, Randbedingungen, ,</v>
-      </c>
-    </row>
-    <row r="29" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="C29" t="s">
-        <v>14</v>
-      </c>
-      <c r="D29">
-        <v>30</v>
-      </c>
-      <c r="F29" t="str">
-        <f t="shared" si="0"/>
-        <v>30, subsection, 2, Luftwechsel, ,</v>
-      </c>
-    </row>
-    <row r="30" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="C30" t="s">
-        <v>15</v>
-      </c>
-      <c r="D30">
-        <v>30</v>
-      </c>
-      <c r="F30" t="str">
-        <f t="shared" si="0"/>
-        <v>30, subsection, 2, Nutzungszeiten, ,</v>
-      </c>
-    </row>
-    <row r="31" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="C31" t="s">
-        <v>16</v>
-      </c>
-      <c r="D31">
-        <v>30</v>
-      </c>
-      <c r="F31" t="str">
-        <f t="shared" si="0"/>
-        <v>30, subsection, 2, Heizung, ,</v>
-      </c>
-    </row>
-    <row r="32" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="C32" t="s">
-        <v>19</v>
-      </c>
-      <c r="D32">
-        <v>31</v>
-      </c>
-      <c r="F32" t="str">
-        <f t="shared" si="0"/>
-        <v>31, subsection, 2, Beleuchtung, ,</v>
-      </c>
-    </row>
-    <row r="33" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="C33" t="s">
-        <v>20</v>
-      </c>
-      <c r="D33">
-        <v>31</v>
-      </c>
-      <c r="F33" t="str">
-        <f t="shared" si="0"/>
-        <v>31, subsection, 2, Wärmequellen, ,</v>
-      </c>
-    </row>
-    <row r="34" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="C34" t="s">
-        <v>24</v>
-      </c>
-      <c r="D34">
-        <v>35</v>
-      </c>
-      <c r="F34" t="str">
-        <f t="shared" si="0"/>
-        <v>35, subsection, 2, Berechnung / Ergebnisse, ,</v>
-      </c>
-    </row>
-    <row r="35" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B35" t="s">
-        <v>27</v>
-      </c>
-      <c r="D35">
-        <v>38</v>
-      </c>
-      <c r="F35" t="str">
-        <f t="shared" si="0"/>
-        <v>38, section, 1, Zone Technik, ,</v>
-      </c>
-    </row>
-    <row r="36" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="C36" t="s">
-        <v>26</v>
-      </c>
-      <c r="D36">
-        <v>38</v>
-      </c>
-      <c r="F36" t="str">
-        <f t="shared" si="0"/>
-        <v>38, subsection, 2, Geometrie, ,</v>
-      </c>
-    </row>
-    <row r="37" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="C37" t="s">
-        <v>9</v>
-      </c>
-      <c r="D37">
-        <v>39</v>
-      </c>
-      <c r="F37" t="str">
-        <f t="shared" si="0"/>
-        <v>39, subsection, 2, Raumliste, ,</v>
-      </c>
-    </row>
-    <row r="38" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="C38" t="s">
-        <v>13</v>
-      </c>
-      <c r="D38">
-        <v>39</v>
-      </c>
-      <c r="F38" t="str">
-        <f t="shared" si="0"/>
-        <v>39, subsection, 2, Randbedingungen, ,</v>
-      </c>
-    </row>
-    <row r="39" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="C39" t="s">
-        <v>14</v>
-      </c>
-      <c r="D39">
-        <v>39</v>
-      </c>
-      <c r="F39" t="str">
-        <f t="shared" si="0"/>
-        <v>39, subsection, 2, Luftwechsel, ,</v>
-      </c>
-    </row>
-    <row r="40" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="C40" t="s">
-        <v>15</v>
-      </c>
-      <c r="D40">
-        <v>39</v>
-      </c>
-      <c r="F40" t="str">
-        <f t="shared" si="0"/>
-        <v>39, subsection, 2, Nutzungszeiten, ,</v>
-      </c>
-    </row>
-    <row r="41" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="C41" t="s">
-        <v>16</v>
-      </c>
-      <c r="D41">
-        <v>39</v>
-      </c>
-      <c r="F41" t="str">
-        <f t="shared" si="0"/>
-        <v>39, subsection, 2, Heizung, ,</v>
-      </c>
-    </row>
-    <row r="42" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="C42" t="s">
-        <v>19</v>
-      </c>
-      <c r="D42">
-        <v>40</v>
-      </c>
-      <c r="F42" t="str">
-        <f t="shared" si="0"/>
-        <v>40, subsection, 2, Beleuchtung, ,</v>
-      </c>
-    </row>
-    <row r="43" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="C43" t="s">
-        <v>20</v>
-      </c>
-      <c r="D43">
-        <v>40</v>
-      </c>
-      <c r="F43" t="str">
-        <f t="shared" si="0"/>
-        <v>40, subsection, 2, Wärmequellen, ,</v>
-      </c>
-    </row>
-    <row r="44" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="C44" t="s">
-        <v>24</v>
-      </c>
-      <c r="D44">
-        <v>44</v>
-      </c>
-      <c r="F44" t="str">
-        <f t="shared" si="0"/>
-        <v>44, subsection, 2, Berechnung / Ergebnisse, ,</v>
-      </c>
-    </row>
-    <row r="45" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B45" t="s">
-        <v>28</v>
-      </c>
-      <c r="D45">
-        <v>47</v>
-      </c>
-      <c r="F45" t="str">
-        <f t="shared" si="0"/>
-        <v>47, section, 1, Zone Aufenthaltsraum, ,</v>
-      </c>
-    </row>
-    <row r="46" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="C46" t="s">
-        <v>26</v>
-      </c>
-      <c r="D46">
-        <v>47</v>
-      </c>
-      <c r="F46" t="str">
-        <f t="shared" si="0"/>
-        <v>47, subsection, 2, Geometrie, ,</v>
-      </c>
-    </row>
-    <row r="47" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="C47" t="s">
-        <v>9</v>
-      </c>
-      <c r="D47">
-        <v>48</v>
-      </c>
-      <c r="F47" t="str">
-        <f t="shared" si="0"/>
-        <v>48, subsection, 2, Raumliste, ,</v>
-      </c>
-    </row>
-    <row r="48" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="C48" t="s">
-        <v>13</v>
-      </c>
-      <c r="D48">
-        <v>48</v>
-      </c>
-      <c r="F48" t="str">
-        <f t="shared" si="0"/>
-        <v>48, subsection, 2, Randbedingungen, ,</v>
-      </c>
-    </row>
-    <row r="49" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="C49" t="s">
-        <v>14</v>
-      </c>
-      <c r="D49">
-        <v>48</v>
-      </c>
-      <c r="F49" t="str">
-        <f t="shared" si="0"/>
-        <v>48, subsection, 2, Luftwechsel, ,</v>
-      </c>
-    </row>
-    <row r="50" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="C50" t="s">
-        <v>15</v>
-      </c>
-      <c r="D50">
-        <v>48</v>
-      </c>
-      <c r="F50" t="str">
-        <f t="shared" si="0"/>
-        <v>48, subsection, 2, Nutzungszeiten, ,</v>
-      </c>
-    </row>
-    <row r="51" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="C51" t="s">
-        <v>16</v>
-      </c>
-      <c r="D51">
-        <v>48</v>
-      </c>
-      <c r="F51" t="str">
-        <f t="shared" si="0"/>
-        <v>48, subsection, 2, Heizung, ,</v>
-      </c>
-    </row>
-    <row r="52" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="C52" t="s">
-        <v>17</v>
-      </c>
-      <c r="D52">
-        <v>49</v>
-      </c>
-      <c r="F52" t="str">
-        <f t="shared" si="0"/>
-        <v>49, subsection, 2, Kühlung, ,</v>
-      </c>
-    </row>
-    <row r="53" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="C53" t="s">
-        <v>19</v>
-      </c>
-      <c r="D53">
-        <v>49</v>
-      </c>
-      <c r="F53" t="str">
-        <f t="shared" si="0"/>
-        <v>49, subsection, 2, Beleuchtung, ,</v>
-      </c>
-    </row>
-    <row r="54" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="C54" t="s">
-        <v>20</v>
-      </c>
-      <c r="D54">
-        <v>49</v>
-      </c>
-      <c r="F54" t="str">
-        <f t="shared" si="0"/>
-        <v>49, subsection, 2, Wärmequellen, ,</v>
-      </c>
-    </row>
-    <row r="55" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="C55" t="s">
-        <v>24</v>
-      </c>
-      <c r="D55">
-        <v>56</v>
-      </c>
-      <c r="F55" t="str">
-        <f t="shared" si="0"/>
-        <v>56, subsection, 2, Berechnung / Ergebnisse, ,</v>
-      </c>
-    </row>
-    <row r="56" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B56" t="s">
-        <v>29</v>
-      </c>
-      <c r="D56">
-        <v>59</v>
-      </c>
-      <c r="F56" t="str">
-        <f t="shared" si="0"/>
-        <v>59, section, 1, Zone Pfandgutlager, ,</v>
-      </c>
-    </row>
-    <row r="57" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="C57" t="s">
-        <v>26</v>
-      </c>
-      <c r="D57">
-        <v>59</v>
-      </c>
-      <c r="F57" t="str">
-        <f t="shared" si="0"/>
-        <v>59, subsection, 2, Geometrie, ,</v>
-      </c>
-    </row>
-    <row r="58" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="C58" t="s">
-        <v>9</v>
-      </c>
-      <c r="D58">
-        <v>60</v>
-      </c>
-      <c r="F58" t="str">
-        <f t="shared" si="0"/>
-        <v>60, subsection, 2, Raumliste, ,</v>
-      </c>
-    </row>
-    <row r="59" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="C59" t="s">
-        <v>13</v>
-      </c>
-      <c r="D59">
-        <v>60</v>
-      </c>
-      <c r="F59" t="str">
-        <f t="shared" si="0"/>
-        <v>60, subsection, 2, Randbedingungen, ,</v>
-      </c>
-    </row>
-    <row r="60" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="C60" t="s">
-        <v>14</v>
-      </c>
-      <c r="D60">
-        <v>60</v>
-      </c>
-      <c r="F60" t="str">
-        <f t="shared" si="0"/>
-        <v>60, subsection, 2, Luftwechsel, ,</v>
-      </c>
-    </row>
-    <row r="61" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="C61" t="s">
-        <v>15</v>
-      </c>
-      <c r="D61">
-        <v>60</v>
-      </c>
-      <c r="F61" t="str">
-        <f t="shared" si="0"/>
-        <v>60, subsection, 2, Nutzungszeiten, ,</v>
-      </c>
-    </row>
-    <row r="62" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="C62" t="s">
-        <v>16</v>
-      </c>
-      <c r="D62">
-        <v>60</v>
-      </c>
-      <c r="F62" t="str">
-        <f t="shared" si="0"/>
-        <v>60, subsection, 2, Heizung, ,</v>
-      </c>
-    </row>
-    <row r="63" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="C63" t="s">
-        <v>18</v>
-      </c>
-      <c r="D63">
-        <v>61</v>
-      </c>
-      <c r="F63" t="str">
-        <f t="shared" si="0"/>
-        <v>61, subsection, 2, Lüftung, ,</v>
-      </c>
-    </row>
-    <row r="64" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="C64" t="s">
-        <v>19</v>
-      </c>
-      <c r="D64">
-        <v>61</v>
-      </c>
-      <c r="F64" t="str">
-        <f t="shared" si="0"/>
-        <v>61, subsection, 2, Beleuchtung, ,</v>
-      </c>
-    </row>
-    <row r="65" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="C65" t="s">
-        <v>20</v>
-      </c>
-      <c r="D65">
-        <v>61</v>
-      </c>
-      <c r="F65" t="str">
-        <f t="shared" si="0"/>
-        <v>61, subsection, 2, Wärmequellen, ,</v>
-      </c>
-    </row>
-    <row r="66" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="C66" t="s">
-        <v>22</v>
-      </c>
-      <c r="D66">
-        <v>61</v>
-      </c>
-      <c r="F66" t="str">
-        <f t="shared" si="0"/>
-        <v>61, subsection, 2, Gezielter Luftaustausch mit Zone Pfangutlager, ,</v>
-      </c>
-    </row>
-    <row r="67" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="C67" t="s">
-        <v>23</v>
-      </c>
-      <c r="D67">
-        <v>61</v>
-      </c>
-      <c r="F67" t="str">
-        <f t="shared" si="0"/>
-        <v>61, subsection, 2, Konfiguration Lüftungsanlage, ,</v>
-      </c>
-    </row>
-    <row r="68" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="C68" t="s">
-        <v>24</v>
-      </c>
-      <c r="D68">
-        <v>65</v>
-      </c>
-      <c r="F68" t="str">
-        <f t="shared" si="0"/>
-        <v>65, subsection, 2, Berechnung / Ergebnisse, ,</v>
-      </c>
-    </row>
-    <row r="69" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B69" t="s">
-        <v>30</v>
-      </c>
-      <c r="D69">
-        <v>68</v>
-      </c>
-      <c r="F69" t="str">
-        <f t="shared" ref="F69:F129" si="1">CONCATENATE(D69,", ",IF(ISBLANK(A69)=FALSE,A$3,IF(ISBLANK(B69)=FALSE,B$3,C$3)),", ",IF(ISBLANK(A69)=FALSE,0,IF(ISBLANK(B69)=FALSE,1,2)),", ",IF(ISBLANK(A69)=FALSE,A69,IF(ISBLANK(B69)=FALSE,B69,C69)),IF(ISBLANK(D70)=TRUE,",",", ,"))</f>
-        <v>68, section, 1, Zone Aktenraum, ,</v>
-      </c>
-    </row>
-    <row r="70" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="C70" t="s">
-        <v>26</v>
-      </c>
-      <c r="D70">
-        <v>68</v>
-      </c>
-      <c r="F70" t="str">
-        <f t="shared" si="1"/>
-        <v>68, subsection, 2, Geometrie, ,</v>
-      </c>
-    </row>
-    <row r="71" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="C71" t="s">
-        <v>9</v>
-      </c>
-      <c r="D71">
-        <v>69</v>
-      </c>
-      <c r="F71" t="str">
-        <f t="shared" si="1"/>
-        <v>69, subsection, 2, Raumliste, ,</v>
-      </c>
-    </row>
-    <row r="72" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="C72" t="s">
-        <v>13</v>
-      </c>
-      <c r="D72">
-        <v>69</v>
-      </c>
-      <c r="F72" t="str">
-        <f t="shared" si="1"/>
-        <v>69, subsection, 2, Randbedingungen, ,</v>
-      </c>
-    </row>
-    <row r="73" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="C73" t="s">
-        <v>14</v>
-      </c>
-      <c r="D73">
-        <v>69</v>
-      </c>
-      <c r="F73" t="str">
-        <f t="shared" si="1"/>
-        <v>69, subsection, 2, Luftwechsel, ,</v>
-      </c>
-    </row>
-    <row r="74" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="C74" t="s">
-        <v>15</v>
-      </c>
-      <c r="D74">
-        <v>69</v>
-      </c>
-      <c r="F74" t="str">
-        <f t="shared" si="1"/>
-        <v>69, subsection, 2, Nutzungszeiten, ,</v>
-      </c>
-    </row>
-    <row r="75" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="C75" t="s">
-        <v>16</v>
-      </c>
-      <c r="D75">
-        <v>69</v>
-      </c>
-      <c r="F75" t="str">
-        <f t="shared" si="1"/>
-        <v>69, subsection, 2, Heizung, ,</v>
-      </c>
-    </row>
-    <row r="76" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="C76" t="s">
-        <v>17</v>
-      </c>
-      <c r="D76">
-        <v>70</v>
-      </c>
-      <c r="F76" t="str">
-        <f t="shared" si="1"/>
-        <v>70, subsection, 2, Kühlung, ,</v>
-      </c>
-    </row>
-    <row r="77" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="C77" t="s">
-        <v>18</v>
-      </c>
-      <c r="D77">
-        <v>70</v>
-      </c>
-      <c r="F77" t="str">
-        <f t="shared" si="1"/>
-        <v>70, subsection, 2, Lüftung, ,</v>
-      </c>
-    </row>
-    <row r="78" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="C78" t="s">
-        <v>19</v>
-      </c>
-      <c r="D78">
-        <v>70</v>
-      </c>
-      <c r="F78" t="str">
-        <f t="shared" si="1"/>
-        <v>70, subsection, 2, Beleuchtung, ,</v>
-      </c>
-    </row>
-    <row r="79" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="C79" t="s">
-        <v>20</v>
-      </c>
-      <c r="D79">
-        <v>70</v>
-      </c>
-      <c r="F79" t="str">
-        <f t="shared" si="1"/>
-        <v>70, subsection, 2, Wärmequellen, ,</v>
-      </c>
-    </row>
-    <row r="80" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="C80" t="s">
-        <v>23</v>
-      </c>
-      <c r="D80">
-        <v>70</v>
-      </c>
-      <c r="F80" t="str">
-        <f t="shared" si="1"/>
-        <v>70, subsection, 2, Konfiguration Lüftungsanlage, ,</v>
-      </c>
-    </row>
-    <row r="81" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="C81" t="s">
-        <v>24</v>
-      </c>
-      <c r="D81">
-        <v>78</v>
-      </c>
-      <c r="F81" t="str">
-        <f t="shared" si="1"/>
-        <v>78, subsection, 2, Berechnung / Ergebnisse, ,</v>
-      </c>
-    </row>
-    <row r="82" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B82" t="s">
-        <v>31</v>
-      </c>
-      <c r="D82">
-        <v>81</v>
-      </c>
-      <c r="F82" t="str">
-        <f t="shared" si="1"/>
-        <v>81, section, 1, Zone WC, Umkleide, ,</v>
-      </c>
-    </row>
-    <row r="83" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="C83" t="s">
-        <v>26</v>
-      </c>
-      <c r="D83">
-        <v>81</v>
-      </c>
-      <c r="F83" t="str">
-        <f t="shared" si="1"/>
-        <v>81, subsection, 2, Geometrie, ,</v>
-      </c>
-    </row>
-    <row r="84" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="C84" t="s">
-        <v>9</v>
-      </c>
-      <c r="D84">
-        <v>82</v>
-      </c>
-      <c r="F84" t="str">
-        <f t="shared" si="1"/>
-        <v>82, subsection, 2, Raumliste, ,</v>
-      </c>
-    </row>
-    <row r="85" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="C85" t="s">
-        <v>13</v>
-      </c>
-      <c r="D85">
-        <v>82</v>
-      </c>
-      <c r="F85" t="str">
-        <f t="shared" si="1"/>
-        <v>82, subsection, 2, Randbedingungen, ,</v>
-      </c>
-    </row>
-    <row r="86" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="C86" t="s">
-        <v>14</v>
-      </c>
-      <c r="D86">
-        <v>82</v>
-      </c>
-      <c r="F86" t="str">
-        <f t="shared" si="1"/>
-        <v>82, subsection, 2, Luftwechsel, ,</v>
-      </c>
-    </row>
-    <row r="87" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="C87" t="s">
-        <v>15</v>
-      </c>
-      <c r="D87">
-        <v>82</v>
-      </c>
-      <c r="F87" t="str">
-        <f t="shared" si="1"/>
-        <v>82, subsection, 2, Nutzungszeiten, ,</v>
-      </c>
-    </row>
-    <row r="88" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="C88" t="s">
-        <v>16</v>
-      </c>
-      <c r="D88">
-        <v>83</v>
-      </c>
-      <c r="F88" t="str">
-        <f t="shared" si="1"/>
-        <v>83, subsection, 2, Heizung, ,</v>
-      </c>
-    </row>
-    <row r="89" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="C89" t="s">
-        <v>18</v>
-      </c>
-      <c r="D89">
-        <v>83</v>
-      </c>
-      <c r="F89" t="str">
-        <f t="shared" si="1"/>
-        <v>83, subsection, 2, Lüftung, ,</v>
-      </c>
-    </row>
-    <row r="90" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="C90" t="s">
-        <v>19</v>
-      </c>
-      <c r="D90">
-        <v>83</v>
-      </c>
-      <c r="F90" t="str">
-        <f t="shared" si="1"/>
-        <v>83, subsection, 2, Beleuchtung, ,</v>
-      </c>
-    </row>
-    <row r="91" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="C91" t="s">
-        <v>20</v>
-      </c>
-      <c r="D91">
-        <v>83</v>
-      </c>
-      <c r="F91" t="str">
-        <f t="shared" si="1"/>
-        <v>83, subsection, 2, Wärmequellen, ,</v>
-      </c>
-    </row>
-    <row r="92" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="C92" t="s">
-        <v>23</v>
-      </c>
-      <c r="D92">
-        <v>83</v>
-      </c>
-      <c r="F92" t="str">
-        <f t="shared" si="1"/>
-        <v>83, subsection, 2, Konfiguration Lüftungsanlage, ,</v>
-      </c>
-    </row>
-    <row r="93" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="C93" t="s">
-        <v>24</v>
-      </c>
-      <c r="D93">
-        <v>88</v>
-      </c>
-      <c r="F93" t="str">
-        <f t="shared" si="1"/>
-        <v>88, subsection, 2, Berechnung / Ergebnisse, ,</v>
-      </c>
-    </row>
-    <row r="94" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B94" t="s">
-        <v>32</v>
-      </c>
-      <c r="D94">
-        <v>91</v>
-      </c>
-      <c r="F94" t="str">
-        <f t="shared" si="1"/>
-        <v>91, section, 1, Zone RVL Büro, ,</v>
-      </c>
-    </row>
-    <row r="95" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="C95" t="s">
-        <v>26</v>
-      </c>
-      <c r="D95">
-        <v>91</v>
-      </c>
-      <c r="F95" t="str">
-        <f t="shared" si="1"/>
-        <v>91, subsection, 2, Geometrie, ,</v>
-      </c>
-    </row>
-    <row r="96" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="C96" t="s">
-        <v>9</v>
-      </c>
-      <c r="D96">
-        <v>92</v>
-      </c>
-      <c r="F96" t="str">
-        <f t="shared" si="1"/>
-        <v>92, subsection, 2, Raumliste, ,</v>
-      </c>
-    </row>
-    <row r="97" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="C97" t="s">
-        <v>13</v>
-      </c>
-      <c r="D97">
-        <v>92</v>
-      </c>
-      <c r="F97" t="str">
-        <f t="shared" si="1"/>
-        <v>92, subsection, 2, Randbedingungen, ,</v>
-      </c>
-    </row>
-    <row r="98" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="C98" t="s">
-        <v>14</v>
-      </c>
-      <c r="D98">
-        <v>92</v>
-      </c>
-      <c r="F98" t="str">
-        <f t="shared" si="1"/>
-        <v>92, subsection, 2, Luftwechsel, ,</v>
-      </c>
-    </row>
-    <row r="99" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="C99" t="s">
-        <v>15</v>
-      </c>
-      <c r="D99">
-        <v>92</v>
-      </c>
-      <c r="F99" t="str">
-        <f t="shared" si="1"/>
-        <v>92, subsection, 2, Nutzungszeiten, ,</v>
-      </c>
-    </row>
-    <row r="100" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="C100" t="s">
-        <v>16</v>
-      </c>
-      <c r="D100">
-        <v>92</v>
-      </c>
-      <c r="F100" t="str">
-        <f t="shared" si="1"/>
-        <v>92, subsection, 2, Heizung, ,</v>
-      </c>
-    </row>
-    <row r="101" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="C101" t="s">
-        <v>17</v>
-      </c>
-      <c r="D101">
-        <v>93</v>
-      </c>
-      <c r="F101" t="str">
-        <f t="shared" si="1"/>
-        <v>93, subsection, 2, Kühlung, ,</v>
-      </c>
-    </row>
-    <row r="102" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="C102" t="s">
-        <v>19</v>
-      </c>
-      <c r="D102">
-        <v>93</v>
-      </c>
-      <c r="F102" t="str">
-        <f t="shared" si="1"/>
-        <v>93, subsection, 2, Beleuchtung, ,</v>
-      </c>
-    </row>
-    <row r="103" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="C103" t="s">
-        <v>20</v>
-      </c>
-      <c r="D103">
-        <v>93</v>
-      </c>
-      <c r="F103" t="str">
-        <f t="shared" si="1"/>
-        <v>93, subsection, 2, Wärmequellen, ,</v>
-      </c>
-    </row>
-    <row r="104" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="C104" t="s">
-        <v>24</v>
-      </c>
-      <c r="D104">
-        <v>100</v>
-      </c>
-      <c r="F104" t="str">
-        <f t="shared" si="1"/>
-        <v>100, subsection, 2, Berechnung / Ergebnisse, ,</v>
-      </c>
-    </row>
-    <row r="105" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B105" t="s">
-        <v>33</v>
-      </c>
-      <c r="D105">
-        <v>103</v>
-      </c>
-      <c r="F105" t="str">
-        <f t="shared" si="1"/>
-        <v>103, section, 1, Zone Dachraum, ,</v>
-      </c>
-    </row>
-    <row r="106" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="C106" t="s">
-        <v>26</v>
-      </c>
-      <c r="D106">
-        <v>103</v>
-      </c>
-      <c r="F106" t="str">
-        <f t="shared" si="1"/>
-        <v>103, subsection, 2, Geometrie, ,</v>
-      </c>
-    </row>
-    <row r="107" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="C107" t="s">
-        <v>9</v>
-      </c>
-      <c r="D107">
-        <v>104</v>
-      </c>
-      <c r="F107" t="str">
-        <f t="shared" si="1"/>
-        <v>104, subsection, 2, Raumliste, ,</v>
-      </c>
-    </row>
-    <row r="108" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="C108" t="s">
-        <v>13</v>
-      </c>
-      <c r="D108">
-        <v>104</v>
-      </c>
-      <c r="F108" t="str">
-        <f t="shared" si="1"/>
-        <v>104, subsection, 2, Randbedingungen, ,</v>
-      </c>
-    </row>
-    <row r="109" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="C109" t="s">
-        <v>14</v>
-      </c>
-      <c r="D109">
-        <v>104</v>
-      </c>
-      <c r="F109" t="str">
-        <f t="shared" si="1"/>
-        <v>104, subsection, 2, Luftwechsel, ,</v>
-      </c>
-    </row>
-    <row r="110" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="C110" t="s">
-        <v>15</v>
-      </c>
-      <c r="D110">
-        <v>104</v>
-      </c>
-      <c r="F110" t="str">
-        <f t="shared" si="1"/>
-        <v>104, subsection, 2, Nutzungszeiten, ,</v>
-      </c>
-    </row>
-    <row r="111" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="C111" t="s">
-        <v>19</v>
-      </c>
-      <c r="D111">
-        <v>104</v>
-      </c>
-      <c r="F111" t="str">
-        <f t="shared" si="1"/>
-        <v>104, subsection, 2, Beleuchtung, ,</v>
-      </c>
-    </row>
-    <row r="112" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="C112" t="s">
-        <v>20</v>
-      </c>
-      <c r="D112">
-        <v>105</v>
-      </c>
-      <c r="F112" t="str">
-        <f t="shared" si="1"/>
-        <v>105, subsection, 2, Wärmequellen, ,</v>
-      </c>
-    </row>
-    <row r="113" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="C113" t="s">
-        <v>24</v>
-      </c>
-      <c r="D113">
-        <v>106</v>
-      </c>
-      <c r="F113" t="str">
-        <f t="shared" si="1"/>
-        <v>106, subsection, 2, Berechnung / Ergebnisse, ,</v>
-      </c>
-    </row>
-    <row r="114" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B114" t="s">
-        <v>34</v>
-      </c>
-      <c r="D114">
-        <v>108</v>
-      </c>
-      <c r="F114" t="str">
-        <f t="shared" si="1"/>
-        <v>108, section, 1, Anlagentechnik, ,</v>
-      </c>
-    </row>
-    <row r="115" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="C115" t="s">
-        <v>35</v>
-      </c>
-      <c r="D115">
-        <v>108</v>
-      </c>
-      <c r="F115" t="str">
-        <f t="shared" si="1"/>
-        <v>108, subsection, 2, Heizungsanlage, ,</v>
-      </c>
-    </row>
-    <row r="116" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="C116" t="s">
-        <v>36</v>
-      </c>
-      <c r="D116">
-        <v>111</v>
-      </c>
-      <c r="F116" t="str">
-        <f t="shared" si="1"/>
-        <v>111, subsection, 2, Trinkwasseranlage, ,</v>
-      </c>
-    </row>
-    <row r="117" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="C117" t="s">
-        <v>37</v>
-      </c>
-      <c r="D117">
-        <v>112</v>
-      </c>
-      <c r="F117" t="str">
-        <f t="shared" si="1"/>
-        <v>112, subsection, 2, Kühlungsanlage, ,</v>
-      </c>
-    </row>
-    <row r="118" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="C118" t="s">
-        <v>38</v>
-      </c>
-      <c r="D118">
-        <v>114</v>
-      </c>
-      <c r="F118" t="str">
-        <f t="shared" si="1"/>
-        <v>114, subsection, 2, RLT-Anlage, ,</v>
-      </c>
-    </row>
-    <row r="119" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B119" t="s">
-        <v>19</v>
-      </c>
-      <c r="D119">
-        <v>118</v>
-      </c>
-      <c r="F119" t="str">
-        <f t="shared" si="1"/>
-        <v>118, section, 1, Beleuchtung, ,</v>
-      </c>
-    </row>
-    <row r="120" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="C120" t="s">
-        <v>40</v>
-      </c>
-      <c r="D120">
-        <v>118</v>
-      </c>
-      <c r="F120" t="str">
-        <f t="shared" si="1"/>
-        <v>118, subsection, 2, Verkaufsraum, ,</v>
-      </c>
-    </row>
-    <row r="121" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="C121" t="s">
-        <v>51</v>
-      </c>
-      <c r="D121">
-        <v>118</v>
-      </c>
-      <c r="F121" t="str">
-        <f t="shared" si="1"/>
-        <v>118, subsection, 2, Lager, ,</v>
-      </c>
-    </row>
-    <row r="122" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="C122" t="s">
-        <v>41</v>
-      </c>
-      <c r="D122">
-        <v>118</v>
-      </c>
-      <c r="F122" t="str">
-        <f t="shared" si="1"/>
-        <v>118, subsection, 2, Technik, ,</v>
-      </c>
-    </row>
-    <row r="123" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="C123" t="s">
-        <v>42</v>
-      </c>
-      <c r="D123">
-        <v>119</v>
-      </c>
-      <c r="F123" t="str">
-        <f t="shared" si="1"/>
-        <v>119, subsection, 2, Aufenthaltsraum, ,</v>
-      </c>
-    </row>
-    <row r="124" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="C124" t="s">
-        <v>43</v>
-      </c>
-      <c r="D124">
-        <v>119</v>
-      </c>
-      <c r="F124" t="str">
-        <f t="shared" si="1"/>
-        <v>119, subsection, 2, Pfandgutlager, ,</v>
-      </c>
-    </row>
-    <row r="125" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="C125" t="s">
-        <v>44</v>
-      </c>
-      <c r="D125">
-        <v>120</v>
-      </c>
-      <c r="F125" t="str">
-        <f t="shared" si="1"/>
-        <v>120, subsection, 2, Aktenraum, ,</v>
-      </c>
-    </row>
-    <row r="126" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="C126" t="s">
-        <v>45</v>
-      </c>
-      <c r="D126">
-        <v>120</v>
-      </c>
-      <c r="F126" t="str">
-        <f t="shared" si="1"/>
-        <v>120, subsection, 2, WC, Umkleide, ,</v>
-      </c>
-    </row>
-    <row r="127" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="C127" t="s">
-        <v>46</v>
-      </c>
-      <c r="D127">
-        <v>121</v>
-      </c>
-      <c r="F127" t="str">
-        <f t="shared" si="1"/>
-        <v>121, subsection, 2, RVL Büro, ,</v>
-      </c>
-    </row>
-    <row r="128" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="C128" t="s">
-        <v>47</v>
-      </c>
-      <c r="D128">
-        <v>121</v>
-      </c>
-      <c r="F128" t="str">
-        <f t="shared" si="1"/>
-        <v>121, subsection, 2, Dachraum, ,</v>
-      </c>
-    </row>
-    <row r="129" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B129" t="s">
-        <v>48</v>
-      </c>
-      <c r="D129">
-        <v>123</v>
-      </c>
-      <c r="F129" t="str">
-        <f t="shared" si="1"/>
-        <v>123, section, 1, Übersicht der verwendeten Normen und Verordnungen,</v>
+        <v>123, section, 1, {Übersicht der verwendeten Normen und Verordnungen}, a</v>
       </c>
     </row>
   </sheetData>

</xml_diff>